<commit_message>
earning_lyr.m changed to latest_yr.m
</commit_message>
<xml_diff>
--- a/doc/Factor_book-ym-20180518.xlsx
+++ b/doc/Factor_book-ym-20180518.xlsx
@@ -16151,9 +16151,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="37" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -16161,6 +16158,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -16235,22 +16235,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -16261,6 +16252,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -16801,10 +16801,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="178" t="s">
+      <c r="A2" s="181" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="181" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="78" t="s">
@@ -16815,8 +16815,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="178"/>
-      <c r="B3" s="178"/>
+      <c r="A3" s="181"/>
+      <c r="B3" s="181"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -16825,8 +16825,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="178"/>
-      <c r="B4" s="178"/>
+      <c r="A4" s="181"/>
+      <c r="B4" s="181"/>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
@@ -16835,8 +16835,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="178"/>
-      <c r="B5" s="178"/>
+      <c r="A5" s="181"/>
+      <c r="B5" s="181"/>
       <c r="C5" s="78" t="s">
         <v>9</v>
       </c>
@@ -16845,8 +16845,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="178"/>
-      <c r="B6" s="178"/>
+      <c r="A6" s="181"/>
+      <c r="B6" s="181"/>
       <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
@@ -16855,8 +16855,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="178"/>
-      <c r="B7" s="178"/>
+      <c r="A7" s="181"/>
+      <c r="B7" s="181"/>
       <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
@@ -16865,8 +16865,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="178"/>
-      <c r="B8" s="178"/>
+      <c r="A8" s="181"/>
+      <c r="B8" s="181"/>
       <c r="C8" s="78" t="s">
         <v>12</v>
       </c>
@@ -16875,8 +16875,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="178"/>
-      <c r="B9" s="178"/>
+      <c r="A9" s="181"/>
+      <c r="B9" s="181"/>
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
@@ -16885,8 +16885,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="178"/>
-      <c r="B10" s="178"/>
+      <c r="A10" s="181"/>
+      <c r="B10" s="181"/>
       <c r="C10" s="78" t="s">
         <v>14</v>
       </c>
@@ -16895,8 +16895,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="178"/>
-      <c r="B11" s="178"/>
+      <c r="A11" s="181"/>
+      <c r="B11" s="181"/>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -16905,8 +16905,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="178"/>
-      <c r="B12" s="178"/>
+      <c r="A12" s="181"/>
+      <c r="B12" s="181"/>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
@@ -16915,8 +16915,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="178"/>
-      <c r="B13" s="178"/>
+      <c r="A13" s="181"/>
+      <c r="B13" s="181"/>
       <c r="C13" s="78" t="s">
         <v>17</v>
       </c>
@@ -16925,14 +16925,14 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="178"/>
-      <c r="B14" s="179"/>
-      <c r="C14" s="180"/>
-      <c r="D14" s="181"/>
+      <c r="A14" s="181"/>
+      <c r="B14" s="178"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="180"/>
     </row>
     <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="178"/>
-      <c r="B15" s="178" t="s">
+      <c r="A15" s="181"/>
+      <c r="B15" s="181" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -16943,8 +16943,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="178"/>
-      <c r="B16" s="178"/>
+      <c r="A16" s="181"/>
+      <c r="B16" s="181"/>
       <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
@@ -16953,8 +16953,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="178"/>
-      <c r="B17" s="178"/>
+      <c r="A17" s="181"/>
+      <c r="B17" s="181"/>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
@@ -16963,8 +16963,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="178"/>
-      <c r="B18" s="178"/>
+      <c r="A18" s="181"/>
+      <c r="B18" s="181"/>
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
@@ -16973,8 +16973,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="178"/>
-      <c r="B19" s="178"/>
+      <c r="A19" s="181"/>
+      <c r="B19" s="181"/>
       <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
@@ -16983,8 +16983,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="178"/>
-      <c r="B20" s="178"/>
+      <c r="A20" s="181"/>
+      <c r="B20" s="181"/>
       <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
@@ -16993,8 +16993,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="178"/>
-      <c r="B21" s="178"/>
+      <c r="A21" s="181"/>
+      <c r="B21" s="181"/>
       <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
@@ -17003,14 +17003,14 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="178"/>
-      <c r="B22" s="179"/>
-      <c r="C22" s="180"/>
-      <c r="D22" s="181"/>
+      <c r="A22" s="181"/>
+      <c r="B22" s="178"/>
+      <c r="C22" s="179"/>
+      <c r="D22" s="180"/>
     </row>
     <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="178"/>
-      <c r="B23" s="178" t="s">
+      <c r="A23" s="181"/>
+      <c r="B23" s="181" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -17021,8 +17021,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="178"/>
-      <c r="B24" s="178"/>
+      <c r="A24" s="181"/>
+      <c r="B24" s="181"/>
       <c r="C24" s="2" t="s">
         <v>28</v>
       </c>
@@ -17031,8 +17031,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="178"/>
-      <c r="B25" s="178"/>
+      <c r="A25" s="181"/>
+      <c r="B25" s="181"/>
       <c r="C25" s="2" t="s">
         <v>29</v>
       </c>
@@ -17041,8 +17041,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="178"/>
-      <c r="B26" s="178"/>
+      <c r="A26" s="181"/>
+      <c r="B26" s="181"/>
       <c r="C26" s="2" t="s">
         <v>30</v>
       </c>
@@ -17051,8 +17051,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="178"/>
-      <c r="B27" s="178"/>
+      <c r="A27" s="181"/>
+      <c r="B27" s="181"/>
       <c r="C27" s="2" t="s">
         <v>31</v>
       </c>
@@ -17061,8 +17061,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="178"/>
-      <c r="B28" s="178"/>
+      <c r="A28" s="181"/>
+      <c r="B28" s="181"/>
       <c r="C28" s="2" t="s">
         <v>32</v>
       </c>
@@ -17071,8 +17071,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="178"/>
-      <c r="B29" s="178"/>
+      <c r="A29" s="181"/>
+      <c r="B29" s="181"/>
       <c r="C29" s="2" t="s">
         <v>33</v>
       </c>
@@ -17081,8 +17081,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="178"/>
-      <c r="B30" s="178"/>
+      <c r="A30" s="181"/>
+      <c r="B30" s="181"/>
       <c r="C30" s="2" t="s">
         <v>35</v>
       </c>
@@ -17091,8 +17091,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="178"/>
-      <c r="B31" s="178"/>
+      <c r="A31" s="181"/>
+      <c r="B31" s="181"/>
       <c r="C31" s="2" t="s">
         <v>37</v>
       </c>
@@ -17101,8 +17101,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="178"/>
-      <c r="B32" s="178"/>
+      <c r="A32" s="181"/>
+      <c r="B32" s="181"/>
       <c r="C32" s="2" t="s">
         <v>38</v>
       </c>
@@ -17111,8 +17111,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="178"/>
-      <c r="B33" s="178"/>
+      <c r="A33" s="181"/>
+      <c r="B33" s="181"/>
       <c r="C33" s="2" t="s">
         <v>39</v>
       </c>
@@ -17121,8 +17121,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="178"/>
-      <c r="B34" s="178"/>
+      <c r="A34" s="181"/>
+      <c r="B34" s="181"/>
       <c r="C34" s="2" t="s">
         <v>40</v>
       </c>
@@ -17131,14 +17131,14 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A35" s="178"/>
-      <c r="B35" s="179"/>
-      <c r="C35" s="180"/>
-      <c r="D35" s="181"/>
+      <c r="A35" s="181"/>
+      <c r="B35" s="178"/>
+      <c r="C35" s="179"/>
+      <c r="D35" s="180"/>
     </row>
     <row r="36" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="178"/>
-      <c r="B36" s="178" t="s">
+      <c r="A36" s="181"/>
+      <c r="B36" s="181" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -17149,8 +17149,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="178"/>
-      <c r="B37" s="178"/>
+      <c r="A37" s="181"/>
+      <c r="B37" s="181"/>
       <c r="C37" s="2" t="s">
         <v>42</v>
       </c>
@@ -17159,8 +17159,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="178"/>
-      <c r="B38" s="178"/>
+      <c r="A38" s="181"/>
+      <c r="B38" s="181"/>
       <c r="C38" s="2" t="s">
         <v>36</v>
       </c>
@@ -17169,8 +17169,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="178"/>
-      <c r="B39" s="178"/>
+      <c r="A39" s="181"/>
+      <c r="B39" s="181"/>
       <c r="C39" s="2" t="s">
         <v>43</v>
       </c>
@@ -17179,8 +17179,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="178"/>
-      <c r="B40" s="178"/>
+      <c r="A40" s="181"/>
+      <c r="B40" s="181"/>
       <c r="C40" s="2" t="s">
         <v>44</v>
       </c>
@@ -17189,8 +17189,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="178"/>
-      <c r="B41" s="178"/>
+      <c r="A41" s="181"/>
+      <c r="B41" s="181"/>
       <c r="C41" s="2" t="s">
         <v>45</v>
       </c>
@@ -17199,8 +17199,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="178"/>
-      <c r="B42" s="178"/>
+      <c r="A42" s="181"/>
+      <c r="B42" s="181"/>
       <c r="C42" s="2" t="s">
         <v>46</v>
       </c>
@@ -17209,8 +17209,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="178"/>
-      <c r="B43" s="178"/>
+      <c r="A43" s="181"/>
+      <c r="B43" s="181"/>
       <c r="C43" s="2" t="s">
         <v>47</v>
       </c>
@@ -17219,8 +17219,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="178"/>
-      <c r="B44" s="178"/>
+      <c r="A44" s="181"/>
+      <c r="B44" s="181"/>
       <c r="C44" s="2" t="s">
         <v>48</v>
       </c>
@@ -17229,8 +17229,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="178"/>
-      <c r="B45" s="178"/>
+      <c r="A45" s="181"/>
+      <c r="B45" s="181"/>
       <c r="C45" s="2" t="s">
         <v>49</v>
       </c>
@@ -17239,8 +17239,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="178"/>
-      <c r="B46" s="178"/>
+      <c r="A46" s="181"/>
+      <c r="B46" s="181"/>
       <c r="C46" s="2" t="s">
         <v>50</v>
       </c>
@@ -17249,8 +17249,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="178"/>
-      <c r="B47" s="178"/>
+      <c r="A47" s="181"/>
+      <c r="B47" s="181"/>
       <c r="C47" s="2" t="s">
         <v>51</v>
       </c>
@@ -17259,8 +17259,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="178"/>
-      <c r="B48" s="178"/>
+      <c r="A48" s="181"/>
+      <c r="B48" s="181"/>
       <c r="C48" s="2" t="s">
         <v>52</v>
       </c>
@@ -17269,8 +17269,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="178"/>
-      <c r="B49" s="178"/>
+      <c r="A49" s="181"/>
+      <c r="B49" s="181"/>
       <c r="C49" s="2" t="s">
         <v>53</v>
       </c>
@@ -17279,8 +17279,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="178"/>
-      <c r="B50" s="178"/>
+      <c r="A50" s="181"/>
+      <c r="B50" s="181"/>
       <c r="C50" s="2" t="s">
         <v>54</v>
       </c>
@@ -17289,8 +17289,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="178"/>
-      <c r="B51" s="178"/>
+      <c r="A51" s="181"/>
+      <c r="B51" s="181"/>
       <c r="C51" s="2" t="s">
         <v>55</v>
       </c>
@@ -17299,14 +17299,14 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A52" s="178"/>
-      <c r="B52" s="179"/>
-      <c r="C52" s="180"/>
-      <c r="D52" s="181"/>
+      <c r="A52" s="181"/>
+      <c r="B52" s="178"/>
+      <c r="C52" s="179"/>
+      <c r="D52" s="180"/>
     </row>
     <row r="53" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="178"/>
-      <c r="B53" s="178" t="s">
+      <c r="A53" s="181"/>
+      <c r="B53" s="181" t="s">
         <v>56</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -17317,8 +17317,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A54" s="178"/>
-      <c r="B54" s="178"/>
+      <c r="A54" s="181"/>
+      <c r="B54" s="181"/>
       <c r="C54" s="2" t="s">
         <v>58</v>
       </c>
@@ -17327,8 +17327,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A55" s="178"/>
-      <c r="B55" s="178"/>
+      <c r="A55" s="181"/>
+      <c r="B55" s="181"/>
       <c r="C55" s="2" t="s">
         <v>59</v>
       </c>
@@ -17337,8 +17337,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A56" s="178"/>
-      <c r="B56" s="178"/>
+      <c r="A56" s="181"/>
+      <c r="B56" s="181"/>
       <c r="C56" s="2" t="s">
         <v>60</v>
       </c>
@@ -17347,8 +17347,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="178"/>
-      <c r="B57" s="178"/>
+      <c r="A57" s="181"/>
+      <c r="B57" s="181"/>
       <c r="C57" s="2" t="s">
         <v>61</v>
       </c>
@@ -17357,8 +17357,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A58" s="178"/>
-      <c r="B58" s="178"/>
+      <c r="A58" s="181"/>
+      <c r="B58" s="181"/>
       <c r="C58" s="2" t="s">
         <v>62</v>
       </c>
@@ -17367,8 +17367,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="178"/>
-      <c r="B59" s="178"/>
+      <c r="A59" s="181"/>
+      <c r="B59" s="181"/>
       <c r="C59" s="2" t="s">
         <v>63</v>
       </c>
@@ -17377,16 +17377,16 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A60" s="179"/>
-      <c r="B60" s="180"/>
-      <c r="C60" s="180"/>
-      <c r="D60" s="181"/>
+      <c r="A60" s="178"/>
+      <c r="B60" s="179"/>
+      <c r="C60" s="179"/>
+      <c r="D60" s="180"/>
     </row>
     <row r="61" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A61" s="178" t="s">
+      <c r="A61" s="181" t="s">
         <v>64</v>
       </c>
-      <c r="B61" s="178" t="s">
+      <c r="B61" s="181" t="s">
         <v>65</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -17397,8 +17397,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="178"/>
-      <c r="B62" s="178"/>
+      <c r="A62" s="181"/>
+      <c r="B62" s="181"/>
       <c r="C62" s="2" t="s">
         <v>67</v>
       </c>
@@ -17407,8 +17407,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="178"/>
-      <c r="B63" s="178"/>
+      <c r="A63" s="181"/>
+      <c r="B63" s="181"/>
       <c r="C63" s="2" t="s">
         <v>68</v>
       </c>
@@ -17417,8 +17417,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A64" s="178"/>
-      <c r="B64" s="178"/>
+      <c r="A64" s="181"/>
+      <c r="B64" s="181"/>
       <c r="C64" s="2" t="s">
         <v>69</v>
       </c>
@@ -17427,8 +17427,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="178"/>
-      <c r="B65" s="178"/>
+      <c r="A65" s="181"/>
+      <c r="B65" s="181"/>
       <c r="C65" s="2" t="s">
         <v>227</v>
       </c>
@@ -17437,8 +17437,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A66" s="178"/>
-      <c r="B66" s="178"/>
+      <c r="A66" s="181"/>
+      <c r="B66" s="181"/>
       <c r="C66" s="2" t="s">
         <v>228</v>
       </c>
@@ -17447,14 +17447,14 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A67" s="178"/>
-      <c r="B67" s="179"/>
-      <c r="C67" s="180"/>
-      <c r="D67" s="181"/>
+      <c r="A67" s="181"/>
+      <c r="B67" s="178"/>
+      <c r="C67" s="179"/>
+      <c r="D67" s="180"/>
     </row>
     <row r="68" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A68" s="178"/>
-      <c r="B68" s="178" t="s">
+      <c r="A68" s="181"/>
+      <c r="B68" s="181" t="s">
         <v>71</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -17465,8 +17465,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A69" s="178"/>
-      <c r="B69" s="178"/>
+      <c r="A69" s="181"/>
+      <c r="B69" s="181"/>
       <c r="C69" s="2" t="s">
         <v>73</v>
       </c>
@@ -17475,8 +17475,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="178"/>
-      <c r="B70" s="178"/>
+      <c r="A70" s="181"/>
+      <c r="B70" s="181"/>
       <c r="C70" s="2" t="s">
         <v>74</v>
       </c>
@@ -17485,8 +17485,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A71" s="178"/>
-      <c r="B71" s="178"/>
+      <c r="A71" s="181"/>
+      <c r="B71" s="181"/>
       <c r="C71" s="2" t="s">
         <v>75</v>
       </c>
@@ -17495,8 +17495,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A72" s="178"/>
-      <c r="B72" s="178"/>
+      <c r="A72" s="181"/>
+      <c r="B72" s="181"/>
       <c r="C72" s="2" t="s">
         <v>76</v>
       </c>
@@ -17505,8 +17505,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A73" s="178"/>
-      <c r="B73" s="178"/>
+      <c r="A73" s="181"/>
+      <c r="B73" s="181"/>
       <c r="C73" s="2" t="s">
         <v>77</v>
       </c>
@@ -17515,8 +17515,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A74" s="178"/>
-      <c r="B74" s="178"/>
+      <c r="A74" s="181"/>
+      <c r="B74" s="181"/>
       <c r="C74" s="2" t="s">
         <v>78</v>
       </c>
@@ -17525,8 +17525,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A75" s="178"/>
-      <c r="B75" s="178"/>
+      <c r="A75" s="181"/>
+      <c r="B75" s="181"/>
       <c r="C75" s="2" t="s">
         <v>79</v>
       </c>
@@ -17535,8 +17535,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A76" s="178"/>
-      <c r="B76" s="178"/>
+      <c r="A76" s="181"/>
+      <c r="B76" s="181"/>
       <c r="C76" s="2" t="s">
         <v>80</v>
       </c>
@@ -17545,8 +17545,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A77" s="178"/>
-      <c r="B77" s="178"/>
+      <c r="A77" s="181"/>
+      <c r="B77" s="181"/>
       <c r="C77" s="2" t="s">
         <v>81</v>
       </c>
@@ -17555,14 +17555,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A78" s="178"/>
-      <c r="B78" s="179"/>
-      <c r="C78" s="180"/>
-      <c r="D78" s="181"/>
+      <c r="A78" s="181"/>
+      <c r="B78" s="178"/>
+      <c r="C78" s="179"/>
+      <c r="D78" s="180"/>
     </row>
     <row r="79" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A79" s="178"/>
-      <c r="B79" s="178" t="s">
+      <c r="A79" s="181"/>
+      <c r="B79" s="181" t="s">
         <v>82</v>
       </c>
       <c r="C79" s="2" t="s">
@@ -17573,8 +17573,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A80" s="178"/>
-      <c r="B80" s="178"/>
+      <c r="A80" s="181"/>
+      <c r="B80" s="181"/>
       <c r="C80" s="2" t="s">
         <v>84</v>
       </c>
@@ -17583,8 +17583,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A81" s="178"/>
-      <c r="B81" s="178"/>
+      <c r="A81" s="181"/>
+      <c r="B81" s="181"/>
       <c r="C81" s="2" t="s">
         <v>85</v>
       </c>
@@ -17593,8 +17593,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A82" s="178"/>
-      <c r="B82" s="178"/>
+      <c r="A82" s="181"/>
+      <c r="B82" s="181"/>
       <c r="C82" s="2" t="s">
         <v>86</v>
       </c>
@@ -17603,8 +17603,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A83" s="178"/>
-      <c r="B83" s="178"/>
+      <c r="A83" s="181"/>
+      <c r="B83" s="181"/>
       <c r="C83" s="2" t="s">
         <v>87</v>
       </c>
@@ -17613,8 +17613,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A84" s="178"/>
-      <c r="B84" s="178"/>
+      <c r="A84" s="181"/>
+      <c r="B84" s="181"/>
       <c r="C84" s="2" t="s">
         <v>88</v>
       </c>
@@ -17623,14 +17623,14 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A85" s="178"/>
-      <c r="B85" s="179"/>
-      <c r="C85" s="180"/>
-      <c r="D85" s="181"/>
+      <c r="A85" s="181"/>
+      <c r="B85" s="178"/>
+      <c r="C85" s="179"/>
+      <c r="D85" s="180"/>
     </row>
     <row r="86" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A86" s="178"/>
-      <c r="B86" s="178" t="s">
+      <c r="A86" s="181"/>
+      <c r="B86" s="181" t="s">
         <v>89</v>
       </c>
       <c r="C86" s="2" t="s">
@@ -17641,8 +17641,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A87" s="178"/>
-      <c r="B87" s="178"/>
+      <c r="A87" s="181"/>
+      <c r="B87" s="181"/>
       <c r="C87" s="2" t="s">
         <v>91</v>
       </c>
@@ -17651,8 +17651,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A88" s="178"/>
-      <c r="B88" s="178"/>
+      <c r="A88" s="181"/>
+      <c r="B88" s="181"/>
       <c r="C88" s="2" t="s">
         <v>92</v>
       </c>
@@ -17661,8 +17661,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A89" s="178"/>
-      <c r="B89" s="178"/>
+      <c r="A89" s="181"/>
+      <c r="B89" s="181"/>
       <c r="C89" s="2" t="s">
         <v>93</v>
       </c>
@@ -17671,16 +17671,16 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A90" s="179"/>
-      <c r="B90" s="180"/>
-      <c r="C90" s="180"/>
-      <c r="D90" s="181"/>
+      <c r="A90" s="178"/>
+      <c r="B90" s="179"/>
+      <c r="C90" s="179"/>
+      <c r="D90" s="180"/>
     </row>
     <row r="91" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A91" s="178" t="s">
+      <c r="A91" s="181" t="s">
         <v>94</v>
       </c>
-      <c r="B91" s="178" t="s">
+      <c r="B91" s="181" t="s">
         <v>95</v>
       </c>
       <c r="C91" s="2" t="s">
@@ -17691,8 +17691,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A92" s="178"/>
-      <c r="B92" s="178"/>
+      <c r="A92" s="181"/>
+      <c r="B92" s="181"/>
       <c r="C92" s="2" t="s">
         <v>97</v>
       </c>
@@ -17701,8 +17701,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A93" s="178"/>
-      <c r="B93" s="178"/>
+      <c r="A93" s="181"/>
+      <c r="B93" s="181"/>
       <c r="C93" s="2" t="s">
         <v>98</v>
       </c>
@@ -17711,8 +17711,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A94" s="178"/>
-      <c r="B94" s="178"/>
+      <c r="A94" s="181"/>
+      <c r="B94" s="181"/>
       <c r="C94" s="2" t="s">
         <v>99</v>
       </c>
@@ -17721,8 +17721,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A95" s="178"/>
-      <c r="B95" s="178"/>
+      <c r="A95" s="181"/>
+      <c r="B95" s="181"/>
       <c r="C95" s="2" t="s">
         <v>100</v>
       </c>
@@ -17731,8 +17731,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A96" s="178"/>
-      <c r="B96" s="178"/>
+      <c r="A96" s="181"/>
+      <c r="B96" s="181"/>
       <c r="C96" s="2" t="s">
         <v>101</v>
       </c>
@@ -17741,8 +17741,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A97" s="178"/>
-      <c r="B97" s="178"/>
+      <c r="A97" s="181"/>
+      <c r="B97" s="181"/>
       <c r="C97" s="2" t="s">
         <v>102</v>
       </c>
@@ -17751,8 +17751,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A98" s="178"/>
-      <c r="B98" s="178"/>
+      <c r="A98" s="181"/>
+      <c r="B98" s="181"/>
       <c r="C98" s="2" t="s">
         <v>103</v>
       </c>
@@ -17761,8 +17761,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A99" s="178"/>
-      <c r="B99" s="178"/>
+      <c r="A99" s="181"/>
+      <c r="B99" s="181"/>
       <c r="C99" s="2" t="s">
         <v>104</v>
       </c>
@@ -17771,8 +17771,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A100" s="178"/>
-      <c r="B100" s="178"/>
+      <c r="A100" s="181"/>
+      <c r="B100" s="181"/>
       <c r="C100" s="2" t="s">
         <v>105</v>
       </c>
@@ -17781,8 +17781,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A101" s="178"/>
-      <c r="B101" s="178"/>
+      <c r="A101" s="181"/>
+      <c r="B101" s="181"/>
       <c r="C101" s="2" t="s">
         <v>106</v>
       </c>
@@ -17791,8 +17791,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A102" s="178"/>
-      <c r="B102" s="178"/>
+      <c r="A102" s="181"/>
+      <c r="B102" s="181"/>
       <c r="C102" s="2" t="s">
         <v>107</v>
       </c>
@@ -17801,8 +17801,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A103" s="178"/>
-      <c r="B103" s="178"/>
+      <c r="A103" s="181"/>
+      <c r="B103" s="181"/>
       <c r="C103" s="2" t="s">
         <v>108</v>
       </c>
@@ -17811,8 +17811,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A104" s="178"/>
-      <c r="B104" s="178"/>
+      <c r="A104" s="181"/>
+      <c r="B104" s="181"/>
       <c r="C104" s="2" t="s">
         <v>109</v>
       </c>
@@ -17821,8 +17821,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A105" s="178"/>
-      <c r="B105" s="178"/>
+      <c r="A105" s="181"/>
+      <c r="B105" s="181"/>
       <c r="C105" s="2" t="s">
         <v>110</v>
       </c>
@@ -17831,8 +17831,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A106" s="178"/>
-      <c r="B106" s="178"/>
+      <c r="A106" s="181"/>
+      <c r="B106" s="181"/>
       <c r="C106" s="2" t="s">
         <v>111</v>
       </c>
@@ -17841,8 +17841,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A107" s="178"/>
-      <c r="B107" s="178"/>
+      <c r="A107" s="181"/>
+      <c r="B107" s="181"/>
       <c r="C107" s="2" t="s">
         <v>112</v>
       </c>
@@ -17851,8 +17851,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A108" s="178"/>
-      <c r="B108" s="178"/>
+      <c r="A108" s="181"/>
+      <c r="B108" s="181"/>
       <c r="C108" s="2" t="s">
         <v>113</v>
       </c>
@@ -17861,8 +17861,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A109" s="178"/>
-      <c r="B109" s="178"/>
+      <c r="A109" s="181"/>
+      <c r="B109" s="181"/>
       <c r="C109" s="2" t="s">
         <v>114</v>
       </c>
@@ -17871,8 +17871,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A110" s="178"/>
-      <c r="B110" s="178"/>
+      <c r="A110" s="181"/>
+      <c r="B110" s="181"/>
       <c r="C110" s="2" t="s">
         <v>115</v>
       </c>
@@ -17881,16 +17881,16 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A111" s="179"/>
-      <c r="B111" s="180"/>
-      <c r="C111" s="180"/>
-      <c r="D111" s="181"/>
+      <c r="A111" s="178"/>
+      <c r="B111" s="179"/>
+      <c r="C111" s="179"/>
+      <c r="D111" s="180"/>
     </row>
     <row r="112" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A112" s="178" t="s">
+      <c r="A112" s="181" t="s">
         <v>116</v>
       </c>
-      <c r="B112" s="178" t="s">
+      <c r="B112" s="181" t="s">
         <v>116</v>
       </c>
       <c r="C112" s="2" t="s">
@@ -17901,8 +17901,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A113" s="178"/>
-      <c r="B113" s="178"/>
+      <c r="A113" s="181"/>
+      <c r="B113" s="181"/>
       <c r="C113" s="2" t="s">
         <v>118</v>
       </c>
@@ -17911,8 +17911,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A114" s="178"/>
-      <c r="B114" s="178"/>
+      <c r="A114" s="181"/>
+      <c r="B114" s="181"/>
       <c r="C114" s="2" t="s">
         <v>119</v>
       </c>
@@ -17921,8 +17921,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A115" s="178"/>
-      <c r="B115" s="178"/>
+      <c r="A115" s="181"/>
+      <c r="B115" s="181"/>
       <c r="C115" s="2" t="s">
         <v>120</v>
       </c>
@@ -17931,8 +17931,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A116" s="178"/>
-      <c r="B116" s="178"/>
+      <c r="A116" s="181"/>
+      <c r="B116" s="181"/>
       <c r="C116" s="2" t="s">
         <v>121</v>
       </c>
@@ -17941,8 +17941,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A117" s="178"/>
-      <c r="B117" s="178"/>
+      <c r="A117" s="181"/>
+      <c r="B117" s="181"/>
       <c r="C117" s="2" t="s">
         <v>122</v>
       </c>
@@ -17952,6 +17952,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B112:B117"/>
+    <mergeCell ref="A91:A110"/>
+    <mergeCell ref="A112:A117"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="A61:A89"/>
+    <mergeCell ref="B68:B77"/>
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="B91:B110"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B61:B66"/>
     <mergeCell ref="A60:D60"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A111:D111"/>
@@ -17965,18 +17977,6 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B112:B117"/>
-    <mergeCell ref="A91:A110"/>
-    <mergeCell ref="A112:A117"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="A61:A89"/>
-    <mergeCell ref="B68:B77"/>
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="B91:B110"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B61:B66"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19520,7 +19520,7 @@
       <c r="D31" s="55"/>
     </row>
     <row r="33" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A33" s="209" t="s">
+      <c r="A33" s="206" t="s">
         <v>1040</v>
       </c>
       <c r="B33" s="49" t="s">
@@ -19534,7 +19534,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="210"/>
+      <c r="A34" s="208"/>
       <c r="B34" s="19" t="s">
         <v>1026</v>
       </c>
@@ -19542,7 +19542,7 @@
       <c r="D34" s="52"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="210"/>
+      <c r="A35" s="208"/>
       <c r="B35" s="19" t="s">
         <v>1027</v>
       </c>
@@ -19550,7 +19550,7 @@
       <c r="D35" s="52"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="210"/>
+      <c r="A36" s="208"/>
       <c r="B36" s="19" t="s">
         <v>1028</v>
       </c>
@@ -19558,7 +19558,7 @@
       <c r="D36" s="52"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="210"/>
+      <c r="A37" s="208"/>
       <c r="B37" s="19" t="s">
         <v>998</v>
       </c>
@@ -19566,7 +19566,7 @@
       <c r="D37" s="52"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="211"/>
+      <c r="A38" s="207"/>
       <c r="B38" s="54" t="s">
         <v>1028</v>
       </c>
@@ -19574,7 +19574,7 @@
       <c r="D38" s="55"/>
     </row>
     <row r="40" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="209" t="s">
+      <c r="A40" s="206" t="s">
         <v>1042</v>
       </c>
       <c r="B40" s="49" t="s">
@@ -19586,7 +19586,7 @@
       <c r="D40" s="50"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="211"/>
+      <c r="A41" s="207"/>
       <c r="B41" s="54" t="s">
         <v>1030</v>
       </c>
@@ -19599,7 +19599,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A44" s="209" t="s">
+      <c r="A44" s="206" t="s">
         <v>1044</v>
       </c>
       <c r="B44" s="49" t="s">
@@ -19613,7 +19613,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="210"/>
+      <c r="A45" s="208"/>
       <c r="B45" s="19" t="s">
         <v>1032</v>
       </c>
@@ -19621,7 +19621,7 @@
       <c r="D45" s="52"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="210"/>
+      <c r="A46" s="208"/>
       <c r="B46" s="19" t="s">
         <v>1033</v>
       </c>
@@ -19629,7 +19629,7 @@
       <c r="D46" s="52"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="210"/>
+      <c r="A47" s="208"/>
       <c r="B47" s="19" t="s">
         <v>1034</v>
       </c>
@@ -19637,7 +19637,7 @@
       <c r="D47" s="52"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="210"/>
+      <c r="A48" s="208"/>
       <c r="B48" s="19" t="s">
         <v>1035</v>
       </c>
@@ -19645,7 +19645,7 @@
       <c r="D48" s="52"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="210"/>
+      <c r="A49" s="208"/>
       <c r="B49" s="19" t="s">
         <v>1036</v>
       </c>
@@ -19653,7 +19653,7 @@
       <c r="D49" s="52"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="211"/>
+      <c r="A50" s="207"/>
       <c r="B50" s="54"/>
       <c r="C50" s="54"/>
       <c r="D50" s="55"/>
@@ -19714,7 +19714,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="148.5" x14ac:dyDescent="0.15">
-      <c r="A59" s="212" t="s">
+      <c r="A59" s="209" t="s">
         <v>419</v>
       </c>
       <c r="B59" s="49" t="s">
@@ -19728,7 +19728,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="213"/>
+      <c r="A60" s="210"/>
       <c r="B60" s="19" t="s">
         <v>1055</v>
       </c>
@@ -19736,7 +19736,7 @@
       <c r="D60" s="52"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="214"/>
+      <c r="A61" s="211"/>
       <c r="B61" s="54" t="s">
         <v>1056</v>
       </c>
@@ -19908,7 +19908,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A82" s="206" t="s">
+      <c r="A82" s="212" t="s">
         <v>1091</v>
       </c>
       <c r="B82" s="49" t="s">
@@ -19922,7 +19922,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A83" s="207"/>
+      <c r="A83" s="213"/>
       <c r="B83" s="19" t="s">
         <v>1093</v>
       </c>
@@ -19930,7 +19930,7 @@
       <c r="D83" s="52"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A84" s="207"/>
+      <c r="A84" s="213"/>
       <c r="B84" s="19" t="s">
         <v>1094</v>
       </c>
@@ -19938,7 +19938,7 @@
       <c r="D84" s="52"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A85" s="208"/>
+      <c r="A85" s="214"/>
       <c r="B85" s="54" t="s">
         <v>1095</v>
       </c>
@@ -19946,7 +19946,7 @@
       <c r="D85" s="55"/>
     </row>
     <row r="87" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="206" t="s">
+      <c r="A87" s="212" t="s">
         <v>1101</v>
       </c>
       <c r="B87" s="49" t="s">
@@ -19960,7 +19960,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A88" s="207"/>
+      <c r="A88" s="213"/>
       <c r="B88" s="19" t="s">
         <v>1103</v>
       </c>
@@ -19972,7 +19972,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A89" s="207"/>
+      <c r="A89" s="213"/>
       <c r="B89" s="19" t="s">
         <v>1104</v>
       </c>
@@ -19984,7 +19984,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A90" s="207"/>
+      <c r="A90" s="213"/>
       <c r="B90" s="19" t="s">
         <v>1103</v>
       </c>
@@ -19996,7 +19996,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A91" s="207"/>
+      <c r="A91" s="213"/>
       <c r="B91" s="19" t="s">
         <v>1105</v>
       </c>
@@ -20006,7 +20006,7 @@
       <c r="D91" s="52"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A92" s="207"/>
+      <c r="A92" s="213"/>
       <c r="B92" s="19" t="s">
         <v>1103</v>
       </c>
@@ -20014,7 +20014,7 @@
       <c r="D92" s="52"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A93" s="207"/>
+      <c r="A93" s="213"/>
       <c r="B93" s="19" t="s">
         <v>536</v>
       </c>
@@ -20022,7 +20022,7 @@
       <c r="D93" s="52"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A94" s="207"/>
+      <c r="A94" s="213"/>
       <c r="B94" s="19" t="s">
         <v>1106</v>
       </c>
@@ -20030,7 +20030,7 @@
       <c r="D94" s="52"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A95" s="208"/>
+      <c r="A95" s="214"/>
       <c r="B95" s="54" t="s">
         <v>1107</v>
       </c>
@@ -20038,7 +20038,7 @@
       <c r="D95" s="55"/>
     </row>
     <row r="97" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="209" t="s">
+      <c r="A97" s="206" t="s">
         <v>1114</v>
       </c>
       <c r="B97" s="65" t="s">
@@ -20050,7 +20050,7 @@
       <c r="D97" s="66"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A98" s="210"/>
+      <c r="A98" s="208"/>
       <c r="B98" s="67" t="s">
         <v>1115</v>
       </c>
@@ -20060,7 +20060,7 @@
       <c r="D98" s="68"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A99" s="210"/>
+      <c r="A99" s="208"/>
       <c r="B99" s="67" t="s">
         <v>1104</v>
       </c>
@@ -20070,7 +20070,7 @@
       <c r="D99" s="68"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A100" s="210"/>
+      <c r="A100" s="208"/>
       <c r="B100" s="67" t="s">
         <v>1115</v>
       </c>
@@ -20080,7 +20080,7 @@
       <c r="D100" s="68"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A101" s="210"/>
+      <c r="A101" s="208"/>
       <c r="B101" s="67" t="s">
         <v>1105</v>
       </c>
@@ -20090,7 +20090,7 @@
       <c r="D101" s="68"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A102" s="211"/>
+      <c r="A102" s="207"/>
       <c r="B102" s="69" t="s">
         <v>1115</v>
       </c>
@@ -20150,22 +20150,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A87:A95"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A105:A109"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A70:A73"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A33:A38"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A75:A79"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="A87:A95"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A105:A109"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21354,7 +21354,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="209" t="s">
+      <c r="A125" s="206" t="s">
         <v>1312</v>
       </c>
       <c r="B125" s="48" t="s">
@@ -21365,21 +21365,21 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A126" s="210"/>
+      <c r="A126" s="208"/>
       <c r="B126" s="51"/>
       <c r="C126" s="52" t="s">
         <v>1315</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A127" s="210"/>
+      <c r="A127" s="208"/>
       <c r="B127" s="53"/>
       <c r="C127" s="55" t="s">
         <v>1316</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A128" s="210"/>
+      <c r="A128" s="208"/>
       <c r="B128" s="19" t="s">
         <v>1127</v>
       </c>
@@ -21388,7 +21388,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A129" s="210"/>
+      <c r="A129" s="208"/>
       <c r="B129" s="48" t="s">
         <v>717</v>
       </c>
@@ -21397,14 +21397,14 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A130" s="210"/>
+      <c r="A130" s="208"/>
       <c r="B130" s="53"/>
       <c r="C130" s="55" t="s">
         <v>1319</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A131" s="210"/>
+      <c r="A131" s="208"/>
       <c r="B131" s="48" t="s">
         <v>809</v>
       </c>
@@ -21413,14 +21413,14 @@
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A132" s="210"/>
+      <c r="A132" s="208"/>
       <c r="B132" s="53"/>
       <c r="C132" s="55" t="s">
         <v>1321</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A133" s="211"/>
+      <c r="A133" s="207"/>
       <c r="B133" s="54" t="s">
         <v>1322</v>
       </c>
@@ -39968,9 +39968,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+    <sheetView showFormulas="1" tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -40000,7 +40000,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="178" t="s">
+      <c r="A2" s="181" t="s">
         <v>269</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -40020,7 +40020,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="178"/>
+      <c r="A3" s="181"/>
       <c r="B3" s="173" t="s">
         <v>6</v>
       </c>
@@ -40036,7 +40036,7 @@
       <c r="F3" s="111"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="178"/>
+      <c r="A4" s="181"/>
       <c r="B4" s="171" t="s">
         <v>274</v>
       </c>
@@ -40051,7 +40051,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="178"/>
+      <c r="A5" s="181"/>
       <c r="B5" s="172" t="s">
         <v>276</v>
       </c>
@@ -40069,7 +40069,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="178"/>
+      <c r="A6" s="181"/>
       <c r="B6" s="173" t="s">
         <v>9</v>
       </c>
@@ -40087,7 +40087,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="178"/>
+      <c r="A7" s="181"/>
       <c r="B7" s="173" t="s">
         <v>279</v>
       </c>
@@ -40105,7 +40105,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="178"/>
+      <c r="A8" s="181"/>
       <c r="B8" s="17" t="s">
         <v>8</v>
       </c>
@@ -40120,7 +40120,7 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="178"/>
+      <c r="A9" s="181"/>
       <c r="B9" s="173" t="s">
         <v>282</v>
       </c>
@@ -40144,11 +40144,11 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A10" s="179"/>
-      <c r="B10" s="180"/>
-      <c r="C10" s="180"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="181"/>
+      <c r="A10" s="178"/>
+      <c r="B10" s="179"/>
+      <c r="C10" s="179"/>
+      <c r="D10" s="179"/>
+      <c r="E10" s="180"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="185" t="s">
@@ -40273,14 +40273,14 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A18" s="179"/>
-      <c r="B18" s="180"/>
-      <c r="C18" s="180"/>
-      <c r="D18" s="180"/>
-      <c r="E18" s="181"/>
+      <c r="A18" s="178"/>
+      <c r="B18" s="179"/>
+      <c r="C18" s="179"/>
+      <c r="D18" s="179"/>
+      <c r="E18" s="180"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="178" t="s">
+      <c r="A19" s="181" t="s">
         <v>287</v>
       </c>
       <c r="B19" s="173" t="s">
@@ -40300,7 +40300,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="178"/>
+      <c r="A20" s="181"/>
       <c r="B20" s="173" t="s">
         <v>43</v>
       </c>
@@ -40318,7 +40318,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="178"/>
+      <c r="A21" s="181"/>
       <c r="B21" s="173" t="s">
         <v>309</v>
       </c>
@@ -40342,7 +40342,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="178"/>
+      <c r="A22" s="181"/>
       <c r="B22" s="2" t="s">
         <v>311</v>
       </c>
@@ -40360,7 +40360,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="178"/>
+      <c r="A23" s="181"/>
       <c r="B23" s="173" t="s">
         <v>313</v>
       </c>
@@ -40381,7 +40381,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="178"/>
+      <c r="A24" s="181"/>
       <c r="B24" s="173" t="s">
         <v>315</v>
       </c>
@@ -40399,7 +40399,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="178"/>
+      <c r="A25" s="181"/>
       <c r="B25" s="176" t="s">
         <v>317</v>
       </c>
@@ -40415,7 +40415,7 @@
       <c r="F25" s="15"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="178"/>
+      <c r="A26" s="181"/>
       <c r="B26" s="173" t="s">
         <v>319</v>
       </c>
@@ -40436,7 +40436,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="178"/>
+      <c r="A27" s="181"/>
       <c r="B27" s="173" t="s">
         <v>320</v>
       </c>
@@ -40460,11 +40460,11 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.15">
-      <c r="A28" s="179"/>
-      <c r="B28" s="180"/>
-      <c r="C28" s="180"/>
-      <c r="D28" s="180"/>
-      <c r="E28" s="181"/>
+      <c r="A28" s="178"/>
+      <c r="B28" s="179"/>
+      <c r="C28" s="179"/>
+      <c r="D28" s="179"/>
+      <c r="E28" s="180"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="185" t="s">
@@ -40529,11 +40529,11 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="179"/>
-      <c r="B33" s="180"/>
-      <c r="C33" s="180"/>
-      <c r="D33" s="180"/>
-      <c r="E33" s="181"/>
+      <c r="A33" s="178"/>
+      <c r="B33" s="179"/>
+      <c r="C33" s="179"/>
+      <c r="D33" s="179"/>
+      <c r="E33" s="180"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="185" t="s">
@@ -40658,11 +40658,11 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A42" s="179"/>
-      <c r="B42" s="180"/>
-      <c r="C42" s="180"/>
-      <c r="D42" s="180"/>
-      <c r="E42" s="181"/>
+      <c r="A42" s="178"/>
+      <c r="B42" s="179"/>
+      <c r="C42" s="179"/>
+      <c r="D42" s="179"/>
+      <c r="E42" s="180"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="185" t="s">
@@ -40803,17 +40803,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A19:A27"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A34:A41"/>
     <mergeCell ref="A43:A51"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A18:E18"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A42:E42"/>
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A19:A27"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A34:A41"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41404,11 +41404,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A27:D27"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="A10:A15"/>
@@ -41417,6 +41412,11 @@
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A33:A40"/>
     <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A27:D27"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42317,9 +42317,9 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="186"/>
-      <c r="B29" s="179"/>
-      <c r="C29" s="180"/>
-      <c r="D29" s="181"/>
+      <c r="B29" s="178"/>
+      <c r="C29" s="179"/>
+      <c r="D29" s="180"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="186"/>
@@ -42365,9 +42365,9 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="186"/>
-      <c r="B34" s="179"/>
-      <c r="C34" s="180"/>
-      <c r="D34" s="181"/>
+      <c r="B34" s="178"/>
+      <c r="C34" s="179"/>
+      <c r="D34" s="180"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="186"/>
@@ -42463,9 +42463,9 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="186"/>
-      <c r="B44" s="179"/>
-      <c r="C44" s="180"/>
-      <c r="D44" s="181"/>
+      <c r="B44" s="178"/>
+      <c r="C44" s="179"/>
+      <c r="D44" s="180"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="186"/>
@@ -42511,9 +42511,9 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="186"/>
-      <c r="B49" s="179"/>
-      <c r="C49" s="180"/>
-      <c r="D49" s="181"/>
+      <c r="B49" s="178"/>
+      <c r="C49" s="179"/>
+      <c r="D49" s="180"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="186"/>
@@ -42619,14 +42619,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B20:B22"/>
     <mergeCell ref="B24:B28"/>
     <mergeCell ref="A24:A59"/>
     <mergeCell ref="B29:D29"/>
@@ -42637,6 +42629,14 @@
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B50:B59"/>
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
some changes in trading factors
</commit_message>
<xml_diff>
--- a/doc/Factor_book-ym-20180518.xlsx
+++ b/doc/Factor_book-ym-20180518.xlsx
@@ -16207,6 +16207,9 @@
     <xf numFmtId="0" fontId="28" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="37" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -16214,9 +16217,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -16227,24 +16227,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -16258,6 +16240,15 @@
     <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="37" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -16265,6 +16256,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -16330,13 +16330,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -16347,15 +16356,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -16413,7 +16413,7 @@
         <xdr:cNvPr id="7169" name="Text Box 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0700-0000011C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0700-0000011C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -16902,10 +16902,10 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="186" t="s">
+      <c r="A2" s="183" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="186" t="s">
+      <c r="B2" s="183" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="171" t="s">
@@ -16916,8 +16916,8 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="186"/>
-      <c r="B3" s="186"/>
+      <c r="A3" s="183"/>
+      <c r="B3" s="183"/>
       <c r="C3" s="171" t="s">
         <v>7</v>
       </c>
@@ -16926,8 +16926,8 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="186"/>
-      <c r="B4" s="186"/>
+      <c r="A4" s="183"/>
+      <c r="B4" s="183"/>
       <c r="C4" s="171" t="s">
         <v>8</v>
       </c>
@@ -16936,8 +16936,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="186"/>
-      <c r="B5" s="186"/>
+      <c r="A5" s="183"/>
+      <c r="B5" s="183"/>
       <c r="C5" s="171" t="s">
         <v>9</v>
       </c>
@@ -16946,8 +16946,8 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="186"/>
-      <c r="B6" s="186"/>
+      <c r="A6" s="183"/>
+      <c r="B6" s="183"/>
       <c r="C6" s="170" t="s">
         <v>10</v>
       </c>
@@ -16956,8 +16956,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="186"/>
-      <c r="B7" s="186"/>
+      <c r="A7" s="183"/>
+      <c r="B7" s="183"/>
       <c r="C7" s="171" t="s">
         <v>11</v>
       </c>
@@ -16966,8 +16966,8 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="186"/>
-      <c r="B8" s="186"/>
+      <c r="A8" s="183"/>
+      <c r="B8" s="183"/>
       <c r="C8" s="171" t="s">
         <v>12</v>
       </c>
@@ -16976,8 +16976,8 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="186"/>
-      <c r="B9" s="186"/>
+      <c r="A9" s="183"/>
+      <c r="B9" s="183"/>
       <c r="C9" s="171" t="s">
         <v>13</v>
       </c>
@@ -16986,8 +16986,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="186"/>
-      <c r="B10" s="186"/>
+      <c r="A10" s="183"/>
+      <c r="B10" s="183"/>
       <c r="C10" s="170" t="s">
         <v>14</v>
       </c>
@@ -16996,8 +16996,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A11" s="186"/>
-      <c r="B11" s="186"/>
+      <c r="A11" s="183"/>
+      <c r="B11" s="183"/>
       <c r="C11" s="170" t="s">
         <v>15</v>
       </c>
@@ -17006,8 +17006,8 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A12" s="186"/>
-      <c r="B12" s="186"/>
+      <c r="A12" s="183"/>
+      <c r="B12" s="183"/>
       <c r="C12" s="170" t="s">
         <v>16</v>
       </c>
@@ -17016,8 +17016,8 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A13" s="186"/>
-      <c r="B13" s="186"/>
+      <c r="A13" s="183"/>
+      <c r="B13" s="183"/>
       <c r="C13" s="170" t="s">
         <v>17</v>
       </c>
@@ -17026,14 +17026,14 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A14" s="186"/>
-      <c r="B14" s="183"/>
-      <c r="C14" s="184"/>
-      <c r="D14" s="185"/>
+      <c r="A14" s="183"/>
+      <c r="B14" s="184"/>
+      <c r="C14" s="185"/>
+      <c r="D14" s="186"/>
     </row>
     <row r="15" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A15" s="186"/>
-      <c r="B15" s="186" t="s">
+      <c r="A15" s="183"/>
+      <c r="B15" s="183" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -17044,8 +17044,8 @@
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A16" s="186"/>
-      <c r="B16" s="186"/>
+      <c r="A16" s="183"/>
+      <c r="B16" s="183"/>
       <c r="C16" s="2" t="s">
         <v>20</v>
       </c>
@@ -17054,8 +17054,8 @@
       </c>
     </row>
     <row r="17" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A17" s="186"/>
-      <c r="B17" s="186"/>
+      <c r="A17" s="183"/>
+      <c r="B17" s="183"/>
       <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
@@ -17064,8 +17064,8 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A18" s="186"/>
-      <c r="B18" s="186"/>
+      <c r="A18" s="183"/>
+      <c r="B18" s="183"/>
       <c r="C18" s="2" t="s">
         <v>22</v>
       </c>
@@ -17074,8 +17074,8 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A19" s="186"/>
-      <c r="B19" s="186"/>
+      <c r="A19" s="183"/>
+      <c r="B19" s="183"/>
       <c r="C19" s="2" t="s">
         <v>23</v>
       </c>
@@ -17084,8 +17084,8 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A20" s="186"/>
-      <c r="B20" s="186"/>
+      <c r="A20" s="183"/>
+      <c r="B20" s="183"/>
       <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
@@ -17094,8 +17094,8 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A21" s="186"/>
-      <c r="B21" s="186"/>
+      <c r="A21" s="183"/>
+      <c r="B21" s="183"/>
       <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
@@ -17104,14 +17104,14 @@
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A22" s="186"/>
-      <c r="B22" s="183"/>
-      <c r="C22" s="184"/>
-      <c r="D22" s="185"/>
+      <c r="A22" s="183"/>
+      <c r="B22" s="184"/>
+      <c r="C22" s="185"/>
+      <c r="D22" s="186"/>
     </row>
     <row r="23" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A23" s="186"/>
-      <c r="B23" s="186" t="s">
+      <c r="A23" s="183"/>
+      <c r="B23" s="183" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -17122,8 +17122,8 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A24" s="186"/>
-      <c r="B24" s="186"/>
+      <c r="A24" s="183"/>
+      <c r="B24" s="183"/>
       <c r="C24" s="2" t="s">
         <v>28</v>
       </c>
@@ -17132,8 +17132,8 @@
       </c>
     </row>
     <row r="25" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A25" s="186"/>
-      <c r="B25" s="186"/>
+      <c r="A25" s="183"/>
+      <c r="B25" s="183"/>
       <c r="C25" s="2" t="s">
         <v>29</v>
       </c>
@@ -17142,8 +17142,8 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A26" s="186"/>
-      <c r="B26" s="186"/>
+      <c r="A26" s="183"/>
+      <c r="B26" s="183"/>
       <c r="C26" s="2" t="s">
         <v>30</v>
       </c>
@@ -17152,8 +17152,8 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A27" s="186"/>
-      <c r="B27" s="186"/>
+      <c r="A27" s="183"/>
+      <c r="B27" s="183"/>
       <c r="C27" s="2" t="s">
         <v>31</v>
       </c>
@@ -17162,8 +17162,8 @@
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A28" s="186"/>
-      <c r="B28" s="186"/>
+      <c r="A28" s="183"/>
+      <c r="B28" s="183"/>
       <c r="C28" s="2" t="s">
         <v>32</v>
       </c>
@@ -17172,8 +17172,8 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A29" s="186"/>
-      <c r="B29" s="186"/>
+      <c r="A29" s="183"/>
+      <c r="B29" s="183"/>
       <c r="C29" s="2" t="s">
         <v>33</v>
       </c>
@@ -17182,8 +17182,8 @@
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A30" s="186"/>
-      <c r="B30" s="186"/>
+      <c r="A30" s="183"/>
+      <c r="B30" s="183"/>
       <c r="C30" s="2" t="s">
         <v>35</v>
       </c>
@@ -17192,8 +17192,8 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A31" s="186"/>
-      <c r="B31" s="186"/>
+      <c r="A31" s="183"/>
+      <c r="B31" s="183"/>
       <c r="C31" s="2" t="s">
         <v>37</v>
       </c>
@@ -17202,8 +17202,8 @@
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A32" s="186"/>
-      <c r="B32" s="186"/>
+      <c r="A32" s="183"/>
+      <c r="B32" s="183"/>
       <c r="C32" s="2" t="s">
         <v>38</v>
       </c>
@@ -17212,8 +17212,8 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A33" s="186"/>
-      <c r="B33" s="186"/>
+      <c r="A33" s="183"/>
+      <c r="B33" s="183"/>
       <c r="C33" s="2" t="s">
         <v>39</v>
       </c>
@@ -17222,8 +17222,8 @@
       </c>
     </row>
     <row r="34" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A34" s="186"/>
-      <c r="B34" s="186"/>
+      <c r="A34" s="183"/>
+      <c r="B34" s="183"/>
       <c r="C34" s="2" t="s">
         <v>40</v>
       </c>
@@ -17232,14 +17232,14 @@
       </c>
     </row>
     <row r="35" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A35" s="186"/>
-      <c r="B35" s="183"/>
-      <c r="C35" s="184"/>
-      <c r="D35" s="185"/>
+      <c r="A35" s="183"/>
+      <c r="B35" s="184"/>
+      <c r="C35" s="185"/>
+      <c r="D35" s="186"/>
     </row>
     <row r="36" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A36" s="186"/>
-      <c r="B36" s="186" t="s">
+      <c r="A36" s="183"/>
+      <c r="B36" s="183" t="s">
         <v>41</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -17250,8 +17250,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A37" s="186"/>
-      <c r="B37" s="186"/>
+      <c r="A37" s="183"/>
+      <c r="B37" s="183"/>
       <c r="C37" s="2" t="s">
         <v>42</v>
       </c>
@@ -17260,8 +17260,8 @@
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A38" s="186"/>
-      <c r="B38" s="186"/>
+      <c r="A38" s="183"/>
+      <c r="B38" s="183"/>
       <c r="C38" s="2" t="s">
         <v>36</v>
       </c>
@@ -17270,8 +17270,8 @@
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A39" s="186"/>
-      <c r="B39" s="186"/>
+      <c r="A39" s="183"/>
+      <c r="B39" s="183"/>
       <c r="C39" s="2" t="s">
         <v>43</v>
       </c>
@@ -17280,8 +17280,8 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A40" s="186"/>
-      <c r="B40" s="186"/>
+      <c r="A40" s="183"/>
+      <c r="B40" s="183"/>
       <c r="C40" s="2" t="s">
         <v>44</v>
       </c>
@@ -17290,8 +17290,8 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A41" s="186"/>
-      <c r="B41" s="186"/>
+      <c r="A41" s="183"/>
+      <c r="B41" s="183"/>
       <c r="C41" s="2" t="s">
         <v>45</v>
       </c>
@@ -17300,8 +17300,8 @@
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A42" s="186"/>
-      <c r="B42" s="186"/>
+      <c r="A42" s="183"/>
+      <c r="B42" s="183"/>
       <c r="C42" s="2" t="s">
         <v>46</v>
       </c>
@@ -17310,8 +17310,8 @@
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A43" s="186"/>
-      <c r="B43" s="186"/>
+      <c r="A43" s="183"/>
+      <c r="B43" s="183"/>
       <c r="C43" s="2" t="s">
         <v>47</v>
       </c>
@@ -17320,8 +17320,8 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A44" s="186"/>
-      <c r="B44" s="186"/>
+      <c r="A44" s="183"/>
+      <c r="B44" s="183"/>
       <c r="C44" s="2" t="s">
         <v>48</v>
       </c>
@@ -17330,8 +17330,8 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="186"/>
-      <c r="B45" s="186"/>
+      <c r="A45" s="183"/>
+      <c r="B45" s="183"/>
       <c r="C45" s="2" t="s">
         <v>49</v>
       </c>
@@ -17340,8 +17340,8 @@
       </c>
     </row>
     <row r="46" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A46" s="186"/>
-      <c r="B46" s="186"/>
+      <c r="A46" s="183"/>
+      <c r="B46" s="183"/>
       <c r="C46" s="2" t="s">
         <v>50</v>
       </c>
@@ -17350,8 +17350,8 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A47" s="186"/>
-      <c r="B47" s="186"/>
+      <c r="A47" s="183"/>
+      <c r="B47" s="183"/>
       <c r="C47" s="2" t="s">
         <v>51</v>
       </c>
@@ -17360,8 +17360,8 @@
       </c>
     </row>
     <row r="48" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A48" s="186"/>
-      <c r="B48" s="186"/>
+      <c r="A48" s="183"/>
+      <c r="B48" s="183"/>
       <c r="C48" s="2" t="s">
         <v>52</v>
       </c>
@@ -17370,8 +17370,8 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A49" s="186"/>
-      <c r="B49" s="186"/>
+      <c r="A49" s="183"/>
+      <c r="B49" s="183"/>
       <c r="C49" s="2" t="s">
         <v>53</v>
       </c>
@@ -17380,8 +17380,8 @@
       </c>
     </row>
     <row r="50" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="186"/>
-      <c r="B50" s="186"/>
+      <c r="A50" s="183"/>
+      <c r="B50" s="183"/>
       <c r="C50" s="2" t="s">
         <v>54</v>
       </c>
@@ -17390,8 +17390,8 @@
       </c>
     </row>
     <row r="51" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A51" s="186"/>
-      <c r="B51" s="186"/>
+      <c r="A51" s="183"/>
+      <c r="B51" s="183"/>
       <c r="C51" s="2" t="s">
         <v>55</v>
       </c>
@@ -17400,14 +17400,14 @@
       </c>
     </row>
     <row r="52" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A52" s="186"/>
-      <c r="B52" s="183"/>
-      <c r="C52" s="184"/>
-      <c r="D52" s="185"/>
+      <c r="A52" s="183"/>
+      <c r="B52" s="184"/>
+      <c r="C52" s="185"/>
+      <c r="D52" s="186"/>
     </row>
     <row r="53" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A53" s="186"/>
-      <c r="B53" s="186" t="s">
+      <c r="A53" s="183"/>
+      <c r="B53" s="183" t="s">
         <v>56</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -17418,8 +17418,8 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A54" s="186"/>
-      <c r="B54" s="186"/>
+      <c r="A54" s="183"/>
+      <c r="B54" s="183"/>
       <c r="C54" s="2" t="s">
         <v>58</v>
       </c>
@@ -17428,8 +17428,8 @@
       </c>
     </row>
     <row r="55" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A55" s="186"/>
-      <c r="B55" s="186"/>
+      <c r="A55" s="183"/>
+      <c r="B55" s="183"/>
       <c r="C55" s="2" t="s">
         <v>59</v>
       </c>
@@ -17438,8 +17438,8 @@
       </c>
     </row>
     <row r="56" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A56" s="186"/>
-      <c r="B56" s="186"/>
+      <c r="A56" s="183"/>
+      <c r="B56" s="183"/>
       <c r="C56" s="2" t="s">
         <v>60</v>
       </c>
@@ -17448,8 +17448,8 @@
       </c>
     </row>
     <row r="57" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A57" s="186"/>
-      <c r="B57" s="186"/>
+      <c r="A57" s="183"/>
+      <c r="B57" s="183"/>
       <c r="C57" s="2" t="s">
         <v>61</v>
       </c>
@@ -17458,8 +17458,8 @@
       </c>
     </row>
     <row r="58" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A58" s="186"/>
-      <c r="B58" s="186"/>
+      <c r="A58" s="183"/>
+      <c r="B58" s="183"/>
       <c r="C58" s="2" t="s">
         <v>62</v>
       </c>
@@ -17468,8 +17468,8 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A59" s="186"/>
-      <c r="B59" s="186"/>
+      <c r="A59" s="183"/>
+      <c r="B59" s="183"/>
       <c r="C59" s="2" t="s">
         <v>63</v>
       </c>
@@ -17478,16 +17478,16 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A60" s="183"/>
-      <c r="B60" s="184"/>
-      <c r="C60" s="184"/>
-      <c r="D60" s="185"/>
+      <c r="A60" s="184"/>
+      <c r="B60" s="185"/>
+      <c r="C60" s="185"/>
+      <c r="D60" s="186"/>
     </row>
     <row r="61" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A61" s="186" t="s">
+      <c r="A61" s="183" t="s">
         <v>64</v>
       </c>
-      <c r="B61" s="186" t="s">
+      <c r="B61" s="183" t="s">
         <v>65</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -17498,8 +17498,8 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A62" s="186"/>
-      <c r="B62" s="186"/>
+      <c r="A62" s="183"/>
+      <c r="B62" s="183"/>
       <c r="C62" s="2" t="s">
         <v>67</v>
       </c>
@@ -17508,8 +17508,8 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A63" s="186"/>
-      <c r="B63" s="186"/>
+      <c r="A63" s="183"/>
+      <c r="B63" s="183"/>
       <c r="C63" s="2" t="s">
         <v>68</v>
       </c>
@@ -17518,8 +17518,8 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A64" s="186"/>
-      <c r="B64" s="186"/>
+      <c r="A64" s="183"/>
+      <c r="B64" s="183"/>
       <c r="C64" s="2" t="s">
         <v>69</v>
       </c>
@@ -17528,8 +17528,8 @@
       </c>
     </row>
     <row r="65" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A65" s="186"/>
-      <c r="B65" s="186"/>
+      <c r="A65" s="183"/>
+      <c r="B65" s="183"/>
       <c r="C65" s="2" t="s">
         <v>227</v>
       </c>
@@ -17538,8 +17538,8 @@
       </c>
     </row>
     <row r="66" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A66" s="186"/>
-      <c r="B66" s="186"/>
+      <c r="A66" s="183"/>
+      <c r="B66" s="183"/>
       <c r="C66" s="2" t="s">
         <v>228</v>
       </c>
@@ -17548,14 +17548,14 @@
       </c>
     </row>
     <row r="67" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A67" s="186"/>
-      <c r="B67" s="183"/>
-      <c r="C67" s="184"/>
-      <c r="D67" s="185"/>
+      <c r="A67" s="183"/>
+      <c r="B67" s="184"/>
+      <c r="C67" s="185"/>
+      <c r="D67" s="186"/>
     </row>
     <row r="68" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A68" s="186"/>
-      <c r="B68" s="186" t="s">
+      <c r="A68" s="183"/>
+      <c r="B68" s="183" t="s">
         <v>71</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -17566,8 +17566,8 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A69" s="186"/>
-      <c r="B69" s="186"/>
+      <c r="A69" s="183"/>
+      <c r="B69" s="183"/>
       <c r="C69" s="2" t="s">
         <v>73</v>
       </c>
@@ -17576,8 +17576,8 @@
       </c>
     </row>
     <row r="70" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A70" s="186"/>
-      <c r="B70" s="186"/>
+      <c r="A70" s="183"/>
+      <c r="B70" s="183"/>
       <c r="C70" s="2" t="s">
         <v>74</v>
       </c>
@@ -17586,8 +17586,8 @@
       </c>
     </row>
     <row r="71" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A71" s="186"/>
-      <c r="B71" s="186"/>
+      <c r="A71" s="183"/>
+      <c r="B71" s="183"/>
       <c r="C71" s="2" t="s">
         <v>75</v>
       </c>
@@ -17596,8 +17596,8 @@
       </c>
     </row>
     <row r="72" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A72" s="186"/>
-      <c r="B72" s="186"/>
+      <c r="A72" s="183"/>
+      <c r="B72" s="183"/>
       <c r="C72" s="2" t="s">
         <v>76</v>
       </c>
@@ -17606,8 +17606,8 @@
       </c>
     </row>
     <row r="73" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A73" s="186"/>
-      <c r="B73" s="186"/>
+      <c r="A73" s="183"/>
+      <c r="B73" s="183"/>
       <c r="C73" s="2" t="s">
         <v>77</v>
       </c>
@@ -17616,8 +17616,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A74" s="186"/>
-      <c r="B74" s="186"/>
+      <c r="A74" s="183"/>
+      <c r="B74" s="183"/>
       <c r="C74" s="2" t="s">
         <v>78</v>
       </c>
@@ -17626,8 +17626,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A75" s="186"/>
-      <c r="B75" s="186"/>
+      <c r="A75" s="183"/>
+      <c r="B75" s="183"/>
       <c r="C75" s="2" t="s">
         <v>79</v>
       </c>
@@ -17636,8 +17636,8 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A76" s="186"/>
-      <c r="B76" s="186"/>
+      <c r="A76" s="183"/>
+      <c r="B76" s="183"/>
       <c r="C76" s="2" t="s">
         <v>80</v>
       </c>
@@ -17646,8 +17646,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A77" s="186"/>
-      <c r="B77" s="186"/>
+      <c r="A77" s="183"/>
+      <c r="B77" s="183"/>
       <c r="C77" s="2" t="s">
         <v>81</v>
       </c>
@@ -17656,14 +17656,14 @@
       </c>
     </row>
     <row r="78" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A78" s="186"/>
-      <c r="B78" s="183"/>
-      <c r="C78" s="184"/>
-      <c r="D78" s="185"/>
+      <c r="A78" s="183"/>
+      <c r="B78" s="184"/>
+      <c r="C78" s="185"/>
+      <c r="D78" s="186"/>
     </row>
     <row r="79" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A79" s="186"/>
-      <c r="B79" s="186" t="s">
+      <c r="A79" s="183"/>
+      <c r="B79" s="183" t="s">
         <v>82</v>
       </c>
       <c r="C79" s="2" t="s">
@@ -17674,8 +17674,8 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A80" s="186"/>
-      <c r="B80" s="186"/>
+      <c r="A80" s="183"/>
+      <c r="B80" s="183"/>
       <c r="C80" s="2" t="s">
         <v>84</v>
       </c>
@@ -17684,8 +17684,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A81" s="186"/>
-      <c r="B81" s="186"/>
+      <c r="A81" s="183"/>
+      <c r="B81" s="183"/>
       <c r="C81" s="2" t="s">
         <v>85</v>
       </c>
@@ -17694,8 +17694,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A82" s="186"/>
-      <c r="B82" s="186"/>
+      <c r="A82" s="183"/>
+      <c r="B82" s="183"/>
       <c r="C82" s="2" t="s">
         <v>86</v>
       </c>
@@ -17704,8 +17704,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A83" s="186"/>
-      <c r="B83" s="186"/>
+      <c r="A83" s="183"/>
+      <c r="B83" s="183"/>
       <c r="C83" s="2" t="s">
         <v>87</v>
       </c>
@@ -17714,8 +17714,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A84" s="186"/>
-      <c r="B84" s="186"/>
+      <c r="A84" s="183"/>
+      <c r="B84" s="183"/>
       <c r="C84" s="2" t="s">
         <v>88</v>
       </c>
@@ -17724,14 +17724,14 @@
       </c>
     </row>
     <row r="85" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A85" s="186"/>
-      <c r="B85" s="183"/>
-      <c r="C85" s="184"/>
-      <c r="D85" s="185"/>
+      <c r="A85" s="183"/>
+      <c r="B85" s="184"/>
+      <c r="C85" s="185"/>
+      <c r="D85" s="186"/>
     </row>
     <row r="86" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A86" s="186"/>
-      <c r="B86" s="186" t="s">
+      <c r="A86" s="183"/>
+      <c r="B86" s="183" t="s">
         <v>89</v>
       </c>
       <c r="C86" s="2" t="s">
@@ -17742,8 +17742,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A87" s="186"/>
-      <c r="B87" s="186"/>
+      <c r="A87" s="183"/>
+      <c r="B87" s="183"/>
       <c r="C87" s="2" t="s">
         <v>91</v>
       </c>
@@ -17752,8 +17752,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A88" s="186"/>
-      <c r="B88" s="186"/>
+      <c r="A88" s="183"/>
+      <c r="B88" s="183"/>
       <c r="C88" s="2" t="s">
         <v>92</v>
       </c>
@@ -17762,8 +17762,8 @@
       </c>
     </row>
     <row r="89" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A89" s="186"/>
-      <c r="B89" s="186"/>
+      <c r="A89" s="183"/>
+      <c r="B89" s="183"/>
       <c r="C89" s="2" t="s">
         <v>93</v>
       </c>
@@ -17772,16 +17772,16 @@
       </c>
     </row>
     <row r="90" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A90" s="183"/>
-      <c r="B90" s="184"/>
-      <c r="C90" s="184"/>
-      <c r="D90" s="185"/>
+      <c r="A90" s="184"/>
+      <c r="B90" s="185"/>
+      <c r="C90" s="185"/>
+      <c r="D90" s="186"/>
     </row>
     <row r="91" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A91" s="186" t="s">
+      <c r="A91" s="183" t="s">
         <v>94</v>
       </c>
-      <c r="B91" s="186" t="s">
+      <c r="B91" s="183" t="s">
         <v>95</v>
       </c>
       <c r="C91" s="2" t="s">
@@ -17792,8 +17792,8 @@
       </c>
     </row>
     <row r="92" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A92" s="186"/>
-      <c r="B92" s="186"/>
+      <c r="A92" s="183"/>
+      <c r="B92" s="183"/>
       <c r="C92" s="2" t="s">
         <v>97</v>
       </c>
@@ -17802,8 +17802,8 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A93" s="186"/>
-      <c r="B93" s="186"/>
+      <c r="A93" s="183"/>
+      <c r="B93" s="183"/>
       <c r="C93" s="2" t="s">
         <v>98</v>
       </c>
@@ -17812,8 +17812,8 @@
       </c>
     </row>
     <row r="94" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A94" s="186"/>
-      <c r="B94" s="186"/>
+      <c r="A94" s="183"/>
+      <c r="B94" s="183"/>
       <c r="C94" s="2" t="s">
         <v>99</v>
       </c>
@@ -17822,8 +17822,8 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A95" s="186"/>
-      <c r="B95" s="186"/>
+      <c r="A95" s="183"/>
+      <c r="B95" s="183"/>
       <c r="C95" s="2" t="s">
         <v>100</v>
       </c>
@@ -17832,8 +17832,8 @@
       </c>
     </row>
     <row r="96" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A96" s="186"/>
-      <c r="B96" s="186"/>
+      <c r="A96" s="183"/>
+      <c r="B96" s="183"/>
       <c r="C96" s="2" t="s">
         <v>101</v>
       </c>
@@ -17842,8 +17842,8 @@
       </c>
     </row>
     <row r="97" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A97" s="186"/>
-      <c r="B97" s="186"/>
+      <c r="A97" s="183"/>
+      <c r="B97" s="183"/>
       <c r="C97" s="2" t="s">
         <v>102</v>
       </c>
@@ -17852,8 +17852,8 @@
       </c>
     </row>
     <row r="98" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A98" s="186"/>
-      <c r="B98" s="186"/>
+      <c r="A98" s="183"/>
+      <c r="B98" s="183"/>
       <c r="C98" s="2" t="s">
         <v>103</v>
       </c>
@@ -17862,8 +17862,8 @@
       </c>
     </row>
     <row r="99" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A99" s="186"/>
-      <c r="B99" s="186"/>
+      <c r="A99" s="183"/>
+      <c r="B99" s="183"/>
       <c r="C99" s="2" t="s">
         <v>104</v>
       </c>
@@ -17872,8 +17872,8 @@
       </c>
     </row>
     <row r="100" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A100" s="186"/>
-      <c r="B100" s="186"/>
+      <c r="A100" s="183"/>
+      <c r="B100" s="183"/>
       <c r="C100" s="2" t="s">
         <v>105</v>
       </c>
@@ -17882,8 +17882,8 @@
       </c>
     </row>
     <row r="101" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A101" s="186"/>
-      <c r="B101" s="186"/>
+      <c r="A101" s="183"/>
+      <c r="B101" s="183"/>
       <c r="C101" s="2" t="s">
         <v>106</v>
       </c>
@@ -17892,8 +17892,8 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A102" s="186"/>
-      <c r="B102" s="186"/>
+      <c r="A102" s="183"/>
+      <c r="B102" s="183"/>
       <c r="C102" s="2" t="s">
         <v>107</v>
       </c>
@@ -17902,8 +17902,8 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A103" s="186"/>
-      <c r="B103" s="186"/>
+      <c r="A103" s="183"/>
+      <c r="B103" s="183"/>
       <c r="C103" s="2" t="s">
         <v>108</v>
       </c>
@@ -17912,8 +17912,8 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A104" s="186"/>
-      <c r="B104" s="186"/>
+      <c r="A104" s="183"/>
+      <c r="B104" s="183"/>
       <c r="C104" s="2" t="s">
         <v>109</v>
       </c>
@@ -17922,8 +17922,8 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A105" s="186"/>
-      <c r="B105" s="186"/>
+      <c r="A105" s="183"/>
+      <c r="B105" s="183"/>
       <c r="C105" s="2" t="s">
         <v>110</v>
       </c>
@@ -17932,8 +17932,8 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A106" s="186"/>
-      <c r="B106" s="186"/>
+      <c r="A106" s="183"/>
+      <c r="B106" s="183"/>
       <c r="C106" s="2" t="s">
         <v>111</v>
       </c>
@@ -17942,8 +17942,8 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A107" s="186"/>
-      <c r="B107" s="186"/>
+      <c r="A107" s="183"/>
+      <c r="B107" s="183"/>
       <c r="C107" s="2" t="s">
         <v>112</v>
       </c>
@@ -17952,8 +17952,8 @@
       </c>
     </row>
     <row r="108" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A108" s="186"/>
-      <c r="B108" s="186"/>
+      <c r="A108" s="183"/>
+      <c r="B108" s="183"/>
       <c r="C108" s="2" t="s">
         <v>113</v>
       </c>
@@ -17962,8 +17962,8 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A109" s="186"/>
-      <c r="B109" s="186"/>
+      <c r="A109" s="183"/>
+      <c r="B109" s="183"/>
       <c r="C109" s="2" t="s">
         <v>114</v>
       </c>
@@ -17972,8 +17972,8 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A110" s="186"/>
-      <c r="B110" s="186"/>
+      <c r="A110" s="183"/>
+      <c r="B110" s="183"/>
       <c r="C110" s="2" t="s">
         <v>115</v>
       </c>
@@ -17982,16 +17982,16 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A111" s="183"/>
-      <c r="B111" s="184"/>
-      <c r="C111" s="184"/>
-      <c r="D111" s="185"/>
+      <c r="A111" s="184"/>
+      <c r="B111" s="185"/>
+      <c r="C111" s="185"/>
+      <c r="D111" s="186"/>
     </row>
     <row r="112" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A112" s="186" t="s">
+      <c r="A112" s="183" t="s">
         <v>116</v>
       </c>
-      <c r="B112" s="186" t="s">
+      <c r="B112" s="183" t="s">
         <v>116</v>
       </c>
       <c r="C112" s="2" t="s">
@@ -18002,8 +18002,8 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A113" s="186"/>
-      <c r="B113" s="186"/>
+      <c r="A113" s="183"/>
+      <c r="B113" s="183"/>
       <c r="C113" s="2" t="s">
         <v>118</v>
       </c>
@@ -18012,8 +18012,8 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A114" s="186"/>
-      <c r="B114" s="186"/>
+      <c r="A114" s="183"/>
+      <c r="B114" s="183"/>
       <c r="C114" s="2" t="s">
         <v>119</v>
       </c>
@@ -18022,8 +18022,8 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A115" s="186"/>
-      <c r="B115" s="186"/>
+      <c r="A115" s="183"/>
+      <c r="B115" s="183"/>
       <c r="C115" s="2" t="s">
         <v>120</v>
       </c>
@@ -18032,8 +18032,8 @@
       </c>
     </row>
     <row r="116" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A116" s="186"/>
-      <c r="B116" s="186"/>
+      <c r="A116" s="183"/>
+      <c r="B116" s="183"/>
       <c r="C116" s="2" t="s">
         <v>121</v>
       </c>
@@ -18042,8 +18042,8 @@
       </c>
     </row>
     <row r="117" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A117" s="186"/>
-      <c r="B117" s="186"/>
+      <c r="A117" s="183"/>
+      <c r="B117" s="183"/>
       <c r="C117" s="2" t="s">
         <v>122</v>
       </c>
@@ -18053,18 +18053,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B112:B117"/>
-    <mergeCell ref="A91:A110"/>
-    <mergeCell ref="A112:A117"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="A61:A89"/>
-    <mergeCell ref="B68:B77"/>
-    <mergeCell ref="B79:B84"/>
-    <mergeCell ref="B86:B89"/>
-    <mergeCell ref="B91:B110"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B61:B66"/>
     <mergeCell ref="A60:D60"/>
     <mergeCell ref="A90:D90"/>
     <mergeCell ref="A111:D111"/>
@@ -18078,6 +18066,18 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B112:B117"/>
+    <mergeCell ref="A91:A110"/>
+    <mergeCell ref="A112:A117"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="A61:A89"/>
+    <mergeCell ref="B68:B77"/>
+    <mergeCell ref="B79:B84"/>
+    <mergeCell ref="B86:B89"/>
+    <mergeCell ref="B91:B110"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B61:B66"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19621,7 +19621,7 @@
       <c r="D31" s="55"/>
     </row>
     <row r="33" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A33" s="224" t="s">
+      <c r="A33" s="227" t="s">
         <v>1039</v>
       </c>
       <c r="B33" s="49" t="s">
@@ -19635,7 +19635,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A34" s="226"/>
+      <c r="A34" s="228"/>
       <c r="B34" s="19" t="s">
         <v>1025</v>
       </c>
@@ -19643,7 +19643,7 @@
       <c r="D34" s="52"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A35" s="226"/>
+      <c r="A35" s="228"/>
       <c r="B35" s="19" t="s">
         <v>1026</v>
       </c>
@@ -19651,7 +19651,7 @@
       <c r="D35" s="52"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A36" s="226"/>
+      <c r="A36" s="228"/>
       <c r="B36" s="19" t="s">
         <v>1027</v>
       </c>
@@ -19659,7 +19659,7 @@
       <c r="D36" s="52"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A37" s="226"/>
+      <c r="A37" s="228"/>
       <c r="B37" s="19" t="s">
         <v>997</v>
       </c>
@@ -19667,7 +19667,7 @@
       <c r="D37" s="52"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="225"/>
+      <c r="A38" s="229"/>
       <c r="B38" s="54" t="s">
         <v>1027</v>
       </c>
@@ -19675,7 +19675,7 @@
       <c r="D38" s="55"/>
     </row>
     <row r="40" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A40" s="224" t="s">
+      <c r="A40" s="227" t="s">
         <v>1041</v>
       </c>
       <c r="B40" s="49" t="s">
@@ -19687,7 +19687,7 @@
       <c r="D40" s="50"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A41" s="225"/>
+      <c r="A41" s="229"/>
       <c r="B41" s="54" t="s">
         <v>1029</v>
       </c>
@@ -19700,7 +19700,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A44" s="224" t="s">
+      <c r="A44" s="227" t="s">
         <v>1043</v>
       </c>
       <c r="B44" s="49" t="s">
@@ -19714,7 +19714,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="226"/>
+      <c r="A45" s="228"/>
       <c r="B45" s="19" t="s">
         <v>1031</v>
       </c>
@@ -19722,7 +19722,7 @@
       <c r="D45" s="52"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A46" s="226"/>
+      <c r="A46" s="228"/>
       <c r="B46" s="19" t="s">
         <v>1032</v>
       </c>
@@ -19730,7 +19730,7 @@
       <c r="D46" s="52"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="226"/>
+      <c r="A47" s="228"/>
       <c r="B47" s="19" t="s">
         <v>1033</v>
       </c>
@@ -19738,7 +19738,7 @@
       <c r="D47" s="52"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A48" s="226"/>
+      <c r="A48" s="228"/>
       <c r="B48" s="19" t="s">
         <v>1034</v>
       </c>
@@ -19746,7 +19746,7 @@
       <c r="D48" s="52"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A49" s="226"/>
+      <c r="A49" s="228"/>
       <c r="B49" s="19" t="s">
         <v>1035</v>
       </c>
@@ -19754,7 +19754,7 @@
       <c r="D49" s="52"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A50" s="225"/>
+      <c r="A50" s="229"/>
       <c r="B50" s="54"/>
       <c r="C50" s="54"/>
       <c r="D50" s="55"/>
@@ -19815,7 +19815,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" ht="148.5" x14ac:dyDescent="0.15">
-      <c r="A59" s="227" t="s">
+      <c r="A59" s="230" t="s">
         <v>418</v>
       </c>
       <c r="B59" s="49" t="s">
@@ -19829,7 +19829,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A60" s="228"/>
+      <c r="A60" s="231"/>
       <c r="B60" s="19" t="s">
         <v>1054</v>
       </c>
@@ -19837,7 +19837,7 @@
       <c r="D60" s="52"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="229"/>
+      <c r="A61" s="232"/>
       <c r="B61" s="54" t="s">
         <v>1055</v>
       </c>
@@ -20009,7 +20009,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="94.5" x14ac:dyDescent="0.15">
-      <c r="A82" s="230" t="s">
+      <c r="A82" s="224" t="s">
         <v>1090</v>
       </c>
       <c r="B82" s="49" t="s">
@@ -20023,7 +20023,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A83" s="231"/>
+      <c r="A83" s="225"/>
       <c r="B83" s="19" t="s">
         <v>1092</v>
       </c>
@@ -20031,7 +20031,7 @@
       <c r="D83" s="52"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A84" s="231"/>
+      <c r="A84" s="225"/>
       <c r="B84" s="19" t="s">
         <v>1093</v>
       </c>
@@ -20039,7 +20039,7 @@
       <c r="D84" s="52"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A85" s="232"/>
+      <c r="A85" s="226"/>
       <c r="B85" s="54" t="s">
         <v>1094</v>
       </c>
@@ -20047,7 +20047,7 @@
       <c r="D85" s="55"/>
     </row>
     <row r="87" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="230" t="s">
+      <c r="A87" s="224" t="s">
         <v>1100</v>
       </c>
       <c r="B87" s="49" t="s">
@@ -20061,7 +20061,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A88" s="231"/>
+      <c r="A88" s="225"/>
       <c r="B88" s="19" t="s">
         <v>1102</v>
       </c>
@@ -20073,7 +20073,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A89" s="231"/>
+      <c r="A89" s="225"/>
       <c r="B89" s="19" t="s">
         <v>1103</v>
       </c>
@@ -20085,7 +20085,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A90" s="231"/>
+      <c r="A90" s="225"/>
       <c r="B90" s="19" t="s">
         <v>1102</v>
       </c>
@@ -20097,7 +20097,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A91" s="231"/>
+      <c r="A91" s="225"/>
       <c r="B91" s="19" t="s">
         <v>1104</v>
       </c>
@@ -20107,7 +20107,7 @@
       <c r="D91" s="52"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A92" s="231"/>
+      <c r="A92" s="225"/>
       <c r="B92" s="19" t="s">
         <v>1102</v>
       </c>
@@ -20115,7 +20115,7 @@
       <c r="D92" s="52"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A93" s="231"/>
+      <c r="A93" s="225"/>
       <c r="B93" s="19" t="s">
         <v>535</v>
       </c>
@@ -20123,7 +20123,7 @@
       <c r="D93" s="52"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A94" s="231"/>
+      <c r="A94" s="225"/>
       <c r="B94" s="19" t="s">
         <v>1105</v>
       </c>
@@ -20131,7 +20131,7 @@
       <c r="D94" s="52"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A95" s="232"/>
+      <c r="A95" s="226"/>
       <c r="B95" s="54" t="s">
         <v>1106</v>
       </c>
@@ -20139,7 +20139,7 @@
       <c r="D95" s="55"/>
     </row>
     <row r="97" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="224" t="s">
+      <c r="A97" s="227" t="s">
         <v>1113</v>
       </c>
       <c r="B97" s="65" t="s">
@@ -20151,7 +20151,7 @@
       <c r="D97" s="66"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A98" s="226"/>
+      <c r="A98" s="228"/>
       <c r="B98" s="67" t="s">
         <v>1114</v>
       </c>
@@ -20161,7 +20161,7 @@
       <c r="D98" s="68"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A99" s="226"/>
+      <c r="A99" s="228"/>
       <c r="B99" s="67" t="s">
         <v>1103</v>
       </c>
@@ -20171,7 +20171,7 @@
       <c r="D99" s="68"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A100" s="226"/>
+      <c r="A100" s="228"/>
       <c r="B100" s="67" t="s">
         <v>1114</v>
       </c>
@@ -20181,7 +20181,7 @@
       <c r="D100" s="68"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A101" s="226"/>
+      <c r="A101" s="228"/>
       <c r="B101" s="67" t="s">
         <v>1104</v>
       </c>
@@ -20191,7 +20191,7 @@
       <c r="D101" s="68"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A102" s="225"/>
+      <c r="A102" s="229"/>
       <c r="B102" s="69" t="s">
         <v>1114</v>
       </c>
@@ -20251,22 +20251,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A75:A79"/>
-    <mergeCell ref="A82:A85"/>
-    <mergeCell ref="A87:A95"/>
-    <mergeCell ref="A97:A102"/>
-    <mergeCell ref="A105:A109"/>
-    <mergeCell ref="A44:A50"/>
-    <mergeCell ref="A52:A56"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A64:A68"/>
-    <mergeCell ref="A70:A73"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A33:A38"/>
+    <mergeCell ref="A44:A50"/>
+    <mergeCell ref="A52:A56"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A64:A68"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A75:A79"/>
+    <mergeCell ref="A82:A85"/>
+    <mergeCell ref="A87:A95"/>
+    <mergeCell ref="A97:A102"/>
+    <mergeCell ref="A105:A109"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21455,7 +21455,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="224" t="s">
+      <c r="A125" s="227" t="s">
         <v>1311</v>
       </c>
       <c r="B125" s="48" t="s">
@@ -21466,21 +21466,21 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A126" s="226"/>
+      <c r="A126" s="228"/>
       <c r="B126" s="51"/>
       <c r="C126" s="52" t="s">
         <v>1314</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A127" s="226"/>
+      <c r="A127" s="228"/>
       <c r="B127" s="53"/>
       <c r="C127" s="55" t="s">
         <v>1315</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A128" s="226"/>
+      <c r="A128" s="228"/>
       <c r="B128" s="19" t="s">
         <v>1126</v>
       </c>
@@ -21489,7 +21489,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A129" s="226"/>
+      <c r="A129" s="228"/>
       <c r="B129" s="48" t="s">
         <v>716</v>
       </c>
@@ -21498,14 +21498,14 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A130" s="226"/>
+      <c r="A130" s="228"/>
       <c r="B130" s="53"/>
       <c r="C130" s="55" t="s">
         <v>1318</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A131" s="226"/>
+      <c r="A131" s="228"/>
       <c r="B131" s="48" t="s">
         <v>808</v>
       </c>
@@ -21514,14 +21514,14 @@
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A132" s="226"/>
+      <c r="A132" s="228"/>
       <c r="B132" s="53"/>
       <c r="C132" s="55" t="s">
         <v>1320</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A133" s="225"/>
+      <c r="A133" s="229"/>
       <c r="B133" s="54" t="s">
         <v>1321</v>
       </c>
@@ -40069,9 +40069,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView showFormulas="1" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+    <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -40102,7 +40102,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="196" t="s">
+      <c r="A2" s="190" t="s">
         <v>269</v>
       </c>
       <c r="B2" s="171" t="s">
@@ -40126,7 +40126,7 @@
       <c r="J2" s="175"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="196"/>
+      <c r="A3" s="190"/>
       <c r="B3" s="171" t="s">
         <v>6</v>
       </c>
@@ -40148,7 +40148,7 @@
       <c r="J3" s="175"/>
     </row>
     <row r="4" spans="1:10" s="180" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="196"/>
+      <c r="A4" s="190"/>
       <c r="B4" s="172" t="s">
         <v>274</v>
       </c>
@@ -40163,7 +40163,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="196"/>
+      <c r="A5" s="190"/>
       <c r="B5" s="171" t="s">
         <v>276</v>
       </c>
@@ -40185,7 +40185,7 @@
       <c r="J5" s="175"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="196"/>
+      <c r="A6" s="190"/>
       <c r="B6" s="171" t="s">
         <v>9</v>
       </c>
@@ -40207,7 +40207,7 @@
       <c r="J6" s="175"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="196"/>
+      <c r="A7" s="190"/>
       <c r="B7" s="171" t="s">
         <v>279</v>
       </c>
@@ -40229,7 +40229,7 @@
       <c r="J7" s="175"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="196"/>
+      <c r="A8" s="190"/>
       <c r="B8" s="171" t="s">
         <v>8</v>
       </c>
@@ -40251,7 +40251,7 @@
       <c r="J8" s="175"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="196"/>
+      <c r="A9" s="190"/>
       <c r="B9" s="171" t="s">
         <v>282</v>
       </c>
@@ -40277,11 +40277,11 @@
       <c r="J9" s="175"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A10" s="193"/>
-      <c r="B10" s="194"/>
-      <c r="C10" s="194"/>
-      <c r="D10" s="194"/>
-      <c r="E10" s="195"/>
+      <c r="A10" s="200"/>
+      <c r="B10" s="201"/>
+      <c r="C10" s="201"/>
+      <c r="D10" s="201"/>
+      <c r="E10" s="202"/>
       <c r="F10" s="175"/>
       <c r="G10" s="175"/>
       <c r="H10" s="175"/>
@@ -40289,7 +40289,7 @@
       <c r="J10" s="175"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="197" t="s">
+      <c r="A11" s="191" t="s">
         <v>283</v>
       </c>
       <c r="B11" s="173" t="s">
@@ -40313,7 +40313,7 @@
       <c r="J11" s="175"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="198"/>
+      <c r="A12" s="192"/>
       <c r="B12" s="173" t="s">
         <v>298</v>
       </c>
@@ -40335,7 +40335,7 @@
       <c r="J12" s="175"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="198"/>
+      <c r="A13" s="192"/>
       <c r="B13" s="173" t="s">
         <v>299</v>
       </c>
@@ -40357,7 +40357,7 @@
       <c r="J13" s="175"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="198"/>
+      <c r="A14" s="192"/>
       <c r="B14" s="173" t="s">
         <v>301</v>
       </c>
@@ -40379,7 +40379,7 @@
       <c r="J14" s="175"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="198"/>
+      <c r="A15" s="192"/>
       <c r="B15" s="173" t="s">
         <v>302</v>
       </c>
@@ -40401,7 +40401,7 @@
       <c r="J15" s="175"/>
     </row>
     <row r="16" spans="1:10" s="181" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="198"/>
+      <c r="A16" s="192"/>
       <c r="B16" s="172" t="s">
         <v>304</v>
       </c>
@@ -40417,7 +40417,7 @@
       <c r="F16" s="180"/>
     </row>
     <row r="17" spans="1:10" s="181" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="199"/>
+      <c r="A17" s="193"/>
       <c r="B17" s="172" t="s">
         <v>306</v>
       </c>
@@ -40433,11 +40433,11 @@
       <c r="F17" s="180"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A18" s="193"/>
-      <c r="B18" s="194"/>
-      <c r="C18" s="194"/>
-      <c r="D18" s="194"/>
-      <c r="E18" s="195"/>
+      <c r="A18" s="200"/>
+      <c r="B18" s="201"/>
+      <c r="C18" s="201"/>
+      <c r="D18" s="201"/>
+      <c r="E18" s="202"/>
       <c r="F18" s="175"/>
       <c r="G18" s="175"/>
       <c r="H18" s="175"/>
@@ -40445,7 +40445,7 @@
       <c r="J18" s="175"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="196" t="s">
+      <c r="A19" s="190" t="s">
         <v>287</v>
       </c>
       <c r="B19" s="171" t="s">
@@ -40471,7 +40471,7 @@
       <c r="J19" s="175"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="196"/>
+      <c r="A20" s="190"/>
       <c r="B20" s="171" t="s">
         <v>43</v>
       </c>
@@ -40495,7 +40495,7 @@
       <c r="J20" s="175"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="196"/>
+      <c r="A21" s="190"/>
       <c r="B21" s="171" t="s">
         <v>309</v>
       </c>
@@ -40519,7 +40519,7 @@
       <c r="J21" s="175"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="196"/>
+      <c r="A22" s="190"/>
       <c r="B22" s="171" t="s">
         <v>311</v>
       </c>
@@ -40543,7 +40543,7 @@
       <c r="J22" s="175"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="196"/>
+      <c r="A23" s="190"/>
       <c r="B23" s="171" t="s">
         <v>313</v>
       </c>
@@ -40567,7 +40567,7 @@
       <c r="J23" s="175"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="196"/>
+      <c r="A24" s="190"/>
       <c r="B24" s="173" t="s">
         <v>315</v>
       </c>
@@ -40591,7 +40591,7 @@
       <c r="J24" s="175"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="196"/>
+      <c r="A25" s="190"/>
       <c r="B25" s="171" t="s">
         <v>316</v>
       </c>
@@ -40615,7 +40615,7 @@
       <c r="J25" s="175"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="196"/>
+      <c r="A26" s="190"/>
       <c r="B26" s="171" t="s">
         <v>318</v>
       </c>
@@ -40639,7 +40639,7 @@
       <c r="J26" s="175"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="196"/>
+      <c r="A27" s="190"/>
       <c r="B27" s="171" t="s">
         <v>319</v>
       </c>
@@ -40667,20 +40667,20 @@
       <c r="J27" s="175"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A28" s="183"/>
-      <c r="B28" s="184"/>
-      <c r="C28" s="184"/>
-      <c r="D28" s="184"/>
-      <c r="E28" s="185"/>
+      <c r="A28" s="184"/>
+      <c r="B28" s="185"/>
+      <c r="C28" s="185"/>
+      <c r="D28" s="185"/>
+      <c r="E28" s="186"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="190" t="s">
+      <c r="A29" s="191" t="s">
         <v>288</v>
       </c>
-      <c r="B29" s="174" t="s">
+      <c r="B29" s="171" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="174" t="s">
+      <c r="C29" s="171" t="s">
         <v>321</v>
       </c>
       <c r="D29" s="174" t="s">
@@ -40691,11 +40691,11 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="191"/>
-      <c r="B30" s="174" t="s">
+      <c r="A30" s="192"/>
+      <c r="B30" s="171" t="s">
         <v>67</v>
       </c>
-      <c r="C30" s="174" t="s">
+      <c r="C30" s="171" t="s">
         <v>322</v>
       </c>
       <c r="D30" s="174" t="s">
@@ -40706,11 +40706,11 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="191"/>
-      <c r="B31" s="174" t="s">
+      <c r="A31" s="192"/>
+      <c r="B31" s="171" t="s">
         <v>323</v>
       </c>
-      <c r="C31" s="174" t="s">
+      <c r="C31" s="171" t="s">
         <v>324</v>
       </c>
       <c r="D31" s="174" t="s">
@@ -40721,11 +40721,11 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="192"/>
-      <c r="B32" s="174" t="s">
+      <c r="A32" s="193"/>
+      <c r="B32" s="171" t="s">
         <v>325</v>
       </c>
-      <c r="C32" s="174" t="s">
+      <c r="C32" s="171" t="s">
         <v>289</v>
       </c>
       <c r="D32" s="174" t="s">
@@ -40736,14 +40736,14 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="175" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="193"/>
-      <c r="B33" s="194"/>
-      <c r="C33" s="194"/>
-      <c r="D33" s="194"/>
-      <c r="E33" s="195"/>
+      <c r="A33" s="200"/>
+      <c r="B33" s="201"/>
+      <c r="C33" s="201"/>
+      <c r="D33" s="201"/>
+      <c r="E33" s="202"/>
     </row>
     <row r="34" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="200" t="s">
+      <c r="A34" s="197" t="s">
         <v>290</v>
       </c>
       <c r="B34" s="172" t="s">
@@ -40766,7 +40766,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="201"/>
+      <c r="A35" s="198"/>
       <c r="B35" s="172" t="s">
         <v>328</v>
       </c>
@@ -40787,7 +40787,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="201"/>
+      <c r="A36" s="198"/>
       <c r="B36" s="172" t="s">
         <v>330</v>
       </c>
@@ -40808,7 +40808,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="201"/>
+      <c r="A37" s="198"/>
       <c r="B37" s="172" t="s">
         <v>332</v>
       </c>
@@ -40829,7 +40829,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="201"/>
+      <c r="A38" s="198"/>
       <c r="B38" s="172" t="s">
         <v>97</v>
       </c>
@@ -40844,7 +40844,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="201"/>
+      <c r="A39" s="198"/>
       <c r="B39" s="172" t="s">
         <v>98</v>
       </c>
@@ -40859,7 +40859,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="201"/>
+      <c r="A40" s="198"/>
       <c r="B40" s="172" t="s">
         <v>334</v>
       </c>
@@ -40880,7 +40880,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="202"/>
+      <c r="A41" s="199"/>
       <c r="B41" s="172" t="s">
         <v>107</v>
       </c>
@@ -40901,14 +40901,14 @@
       </c>
     </row>
     <row r="42" spans="1:7" s="175" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="193"/>
-      <c r="B42" s="194"/>
-      <c r="C42" s="194"/>
-      <c r="D42" s="194"/>
-      <c r="E42" s="195"/>
+      <c r="A42" s="200"/>
+      <c r="B42" s="201"/>
+      <c r="C42" s="201"/>
+      <c r="D42" s="201"/>
+      <c r="E42" s="202"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="190" t="s">
+      <c r="A43" s="194" t="s">
         <v>292</v>
       </c>
       <c r="B43" s="171" t="s">
@@ -40925,11 +40925,11 @@
       </c>
     </row>
     <row r="44" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="191"/>
-      <c r="B44" s="182" t="s">
+      <c r="A44" s="195"/>
+      <c r="B44" s="171" t="s">
         <v>339</v>
       </c>
-      <c r="C44" s="182" t="s">
+      <c r="C44" s="171" t="s">
         <v>340</v>
       </c>
       <c r="D44" s="172" t="s">
@@ -40940,11 +40940,11 @@
       </c>
     </row>
     <row r="45" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="191"/>
-      <c r="B45" s="182" t="s">
+      <c r="A45" s="195"/>
+      <c r="B45" s="171" t="s">
         <v>341</v>
       </c>
-      <c r="C45" s="182" t="s">
+      <c r="C45" s="171" t="s">
         <v>342</v>
       </c>
       <c r="D45" s="172" t="s">
@@ -40955,11 +40955,11 @@
       </c>
     </row>
     <row r="46" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="191"/>
-      <c r="B46" s="182" t="s">
+      <c r="A46" s="195"/>
+      <c r="B46" s="171" t="s">
         <v>343</v>
       </c>
-      <c r="C46" s="182" t="s">
+      <c r="C46" s="171" t="s">
         <v>344</v>
       </c>
       <c r="D46" s="172" t="s">
@@ -40970,7 +40970,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="191"/>
+      <c r="A47" s="195"/>
       <c r="B47" s="182" t="s">
         <v>345</v>
       </c>
@@ -40985,7 +40985,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="191"/>
+      <c r="A48" s="195"/>
       <c r="B48" s="182" t="s">
         <v>347</v>
       </c>
@@ -41000,7 +41000,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="191"/>
+      <c r="A49" s="195"/>
       <c r="B49" s="182" t="s">
         <v>349</v>
       </c>
@@ -41015,7 +41015,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="191"/>
+      <c r="A50" s="195"/>
       <c r="B50" s="182" t="s">
         <v>350</v>
       </c>
@@ -41030,7 +41030,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="192"/>
+      <c r="A51" s="196"/>
       <c r="B51" s="182" t="s">
         <v>352</v>
       </c>
@@ -41046,17 +41046,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="A19:A27"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A34:A41"/>
     <mergeCell ref="A43:A51"/>
     <mergeCell ref="A10:E10"/>
     <mergeCell ref="A18:E18"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A2:A9"/>
+    <mergeCell ref="A11:A17"/>
+    <mergeCell ref="A19:A27"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A34:A41"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -41647,6 +41647,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="A27:D27"/>
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="A10:A15"/>
@@ -41655,11 +41660,6 @@
     <mergeCell ref="A28:A31"/>
     <mergeCell ref="A33:A40"/>
     <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="A27:D27"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -42560,9 +42560,9 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A29" s="204"/>
-      <c r="B29" s="183"/>
-      <c r="C29" s="184"/>
-      <c r="D29" s="185"/>
+      <c r="B29" s="184"/>
+      <c r="C29" s="185"/>
+      <c r="D29" s="186"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="204"/>
@@ -42608,9 +42608,9 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="204"/>
-      <c r="B34" s="183"/>
-      <c r="C34" s="184"/>
-      <c r="D34" s="185"/>
+      <c r="B34" s="184"/>
+      <c r="C34" s="185"/>
+      <c r="D34" s="186"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="204"/>
@@ -42706,9 +42706,9 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="204"/>
-      <c r="B44" s="183"/>
-      <c r="C44" s="184"/>
-      <c r="D44" s="185"/>
+      <c r="B44" s="184"/>
+      <c r="C44" s="185"/>
+      <c r="D44" s="186"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="204"/>
@@ -42754,9 +42754,9 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="204"/>
-      <c r="B49" s="183"/>
-      <c r="C49" s="184"/>
-      <c r="D49" s="185"/>
+      <c r="B49" s="184"/>
+      <c r="C49" s="185"/>
+      <c r="D49" s="186"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="204"/>
@@ -42862,6 +42862,14 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="B2:B8"/>
+    <mergeCell ref="A2:A23"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="B20:B22"/>
     <mergeCell ref="B24:B28"/>
     <mergeCell ref="A24:A59"/>
     <mergeCell ref="B29:D29"/>
@@ -42872,14 +42880,6 @@
     <mergeCell ref="B45:B48"/>
     <mergeCell ref="B49:D49"/>
     <mergeCell ref="B50:B59"/>
-    <mergeCell ref="B2:B8"/>
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="B20:B22"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>